<commit_message>
removing one overlapping ID (keeping Kayna coded, deleting Jared coded)
</commit_message>
<xml_diff>
--- a/correlation_data_full.xlsx
+++ b/correlation_data_full.xlsx
@@ -506,82 +506,82 @@
         </is>
       </c>
       <c r="C2">
-        <v>0.2510642963948749</v>
+        <v>0.2504501141670985</v>
       </c>
       <c r="D2">
-        <v>0.1559033872883254</v>
+        <v>0.1560436763458861</v>
       </c>
       <c r="E2">
-        <v>0.03608637620242932</v>
+        <v>0.0362618943639716</v>
       </c>
       <c r="F2">
-        <v>0.3356007386854665</v>
+        <v>0.3353035436244038</v>
       </c>
       <c r="G2">
-        <v>0.323111317324355</v>
+        <v>0.3236971878390013</v>
       </c>
       <c r="H2">
-        <v>-0.02416373461147085</v>
+        <v>-0.0225201660993329</v>
       </c>
       <c r="I2">
-        <v>0.8961955493199838</v>
+        <v>0.8962132468714507</v>
       </c>
       <c r="J2">
-        <v>0.8869678248564653</v>
+        <v>0.8869066548957314</v>
       </c>
       <c r="K2">
-        <v>0.4924517349744275</v>
+        <v>0.4921262584614316</v>
       </c>
       <c r="L2">
-        <v>0.4806230822728826</v>
+        <v>0.4801512826445933</v>
       </c>
       <c r="M2">
-        <v>0.4215582337954846</v>
+        <v>0.421497118288005</v>
       </c>
       <c r="N2">
-        <v>0.4135082113170079</v>
+        <v>0.4135145171964408</v>
       </c>
       <c r="O2">
-        <v>0.0471792537068802</v>
+        <v>0.04719042423220197</v>
       </c>
       <c r="P2">
-        <v>0.2278437120825874</v>
+        <v>0.2277054854577264</v>
       </c>
       <c r="Q2">
-        <v>0.04392118386067694</v>
+        <v>0.04402615507213722</v>
       </c>
       <c r="R2">
-        <v>0.2223037733492779</v>
+        <v>0.2213858907085259</v>
       </c>
       <c r="S2">
-        <v>0.2051755593973502</v>
+        <v>0.2042195690993944</v>
       </c>
       <c r="T2">
-        <v>0.02379716288421419</v>
+        <v>0.02371808510163974</v>
       </c>
       <c r="U2">
         <v>0.2972912384046406</v>
       </c>
       <c r="V2">
-        <v>0.1864635482265845</v>
+        <v>0.1860749206471915</v>
       </c>
       <c r="W2">
-        <v>0.1854525588369179</v>
+        <v>0.1851961867736124</v>
       </c>
       <c r="X2">
-        <v>0.4140916042283412</v>
+        <v>0.4137782746922496</v>
       </c>
       <c r="Y2">
-        <v>0.4115401023536915</v>
+        <v>0.4121078830032697</v>
       </c>
       <c r="Z2">
-        <v>0.4436045061227945</v>
+        <v>0.4439684890732144</v>
       </c>
       <c r="AA2">
-        <v>0.4395462282622183</v>
+        <v>0.4396399602828737</v>
       </c>
       <c r="AB2">
-        <v>0.462922243465834</v>
+        <v>0.4632929735172144</v>
       </c>
     </row>
     <row r="3">
@@ -591,82 +591,82 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.2510642963948749</v>
+        <v>0.2504501141670985</v>
       </c>
       <c r="D3">
-        <v>0.221987404962807</v>
+        <v>0.2220463438131529</v>
       </c>
       <c r="E3">
-        <v>0.258814109740114</v>
+        <v>0.2589882165716723</v>
       </c>
       <c r="F3">
-        <v>0.3034801346941386</v>
+        <v>0.3032054674842555</v>
       </c>
       <c r="G3">
-        <v>0.3237570419414142</v>
+        <v>0.3239964682391911</v>
       </c>
       <c r="H3">
-        <v>0.050132066623324</v>
+        <v>0.05129771864827716</v>
       </c>
       <c r="I3">
-        <v>0.2555038889054406</v>
+        <v>0.2550760362606682</v>
       </c>
       <c r="J3">
-        <v>0.2360206752074876</v>
+        <v>0.2355100635389874</v>
       </c>
       <c r="K3">
-        <v>0.142226497343822</v>
+        <v>0.1417578490238693</v>
       </c>
       <c r="L3">
-        <v>0.1382328154541606</v>
+        <v>0.1376612696948288</v>
       </c>
       <c r="M3">
-        <v>0.1205740240577348</v>
+        <v>0.1203247618736048</v>
       </c>
       <c r="N3">
-        <v>0.1215203709956318</v>
+        <v>0.1213179227496275</v>
       </c>
       <c r="O3">
-        <v>0.07245568199727372</v>
+        <v>0.07244794954821077</v>
       </c>
       <c r="P3">
-        <v>0.3012398029380268</v>
+        <v>0.3011142612197973</v>
       </c>
       <c r="Q3">
-        <v>0.2372756646158307</v>
+        <v>0.2373910808748982</v>
       </c>
       <c r="R3">
-        <v>0.1712511148831177</v>
+        <v>0.1706431063113516</v>
       </c>
       <c r="S3">
-        <v>0.1975531061210007</v>
+        <v>0.196962808104921</v>
       </c>
       <c r="T3">
-        <v>0.2325718912451744</v>
+        <v>0.2325793648313662</v>
       </c>
       <c r="U3">
         <v>0.3105196320749095</v>
       </c>
       <c r="V3">
-        <v>0.04305032799652037</v>
+        <v>0.04270461594735719</v>
       </c>
       <c r="W3">
-        <v>0.08298519338967646</v>
+        <v>0.08274346329636519</v>
       </c>
       <c r="X3">
-        <v>0.4506063187842265</v>
+        <v>0.4503507050477632</v>
       </c>
       <c r="Y3">
-        <v>0.388035893846712</v>
+        <v>0.3882268416815529</v>
       </c>
       <c r="Z3">
-        <v>0.4463002484186225</v>
+        <v>0.4463879454956496</v>
       </c>
       <c r="AA3">
-        <v>0.4922174989411097</v>
+        <v>0.4921496161070058</v>
       </c>
       <c r="AB3">
-        <v>0.4449190930416342</v>
+        <v>0.4449694344044621</v>
       </c>
     </row>
     <row r="4">
@@ -676,82 +676,82 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.1559033872883254</v>
+        <v>0.1560436763458861</v>
       </c>
       <c r="C4">
-        <v>0.221987404962807</v>
+        <v>0.2220463438131529</v>
       </c>
       <c r="E4">
-        <v>0.8933527529779033</v>
+        <v>0.8933567801407576</v>
       </c>
       <c r="F4">
-        <v>0.1100693107048966</v>
+        <v>0.1101013833874506</v>
       </c>
       <c r="G4">
-        <v>0.06575060002858069</v>
+        <v>0.06573935776970632</v>
       </c>
       <c r="H4">
-        <v>0.191491770102774</v>
+        <v>0.1916488558272403</v>
       </c>
       <c r="I4">
-        <v>0.2257039874244228</v>
+        <v>0.2257782358420033</v>
       </c>
       <c r="J4">
-        <v>0.1694901819227861</v>
+        <v>0.1695741123063069</v>
       </c>
       <c r="K4">
-        <v>-0.01993059353965762</v>
+        <v>-0.01991398570375038</v>
       </c>
       <c r="L4">
-        <v>-0.05656662657225147</v>
+        <v>-0.0565600227370593</v>
       </c>
       <c r="M4">
-        <v>0.2952329416539339</v>
+        <v>0.2952574023671488</v>
       </c>
       <c r="N4">
-        <v>0.2902142175037654</v>
+        <v>0.2902305768007128</v>
       </c>
       <c r="O4">
-        <v>0.283556000835911</v>
+        <v>0.2835567453757912</v>
       </c>
       <c r="P4">
-        <v>0.5460714273553775</v>
+        <v>0.5461144914187797</v>
       </c>
       <c r="Q4">
-        <v>0.5304481930814725</v>
+        <v>0.5304458016652085</v>
       </c>
       <c r="R4">
-        <v>-0.1240975527565239</v>
+        <v>-0.1240677449488455</v>
       </c>
       <c r="S4">
-        <v>-0.07447256535857966</v>
+        <v>-0.07442091165502744</v>
       </c>
       <c r="T4">
-        <v>0.5423124177789915</v>
+        <v>0.5423234575359206</v>
       </c>
       <c r="U4">
         <v>-0.09485279467898015</v>
       </c>
       <c r="V4">
-        <v>0.273645043390364</v>
+        <v>0.2736880457941302</v>
       </c>
       <c r="W4">
-        <v>0.3849021664473969</v>
+        <v>0.3849391823768346</v>
       </c>
       <c r="X4">
-        <v>0.4534135614802932</v>
+        <v>0.4535036178197524</v>
       </c>
       <c r="Y4">
-        <v>0.3380539562958244</v>
+        <v>0.3380533127727982</v>
       </c>
       <c r="Z4">
-        <v>0.4200868156564828</v>
+        <v>0.420085967507008</v>
       </c>
       <c r="AA4">
-        <v>0.4661597273899097</v>
+        <v>0.466173422943744</v>
       </c>
       <c r="AB4">
-        <v>0.4156772580361829</v>
+        <v>0.4156764728076081</v>
       </c>
     </row>
     <row r="5">
@@ -761,82 +761,82 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.03608637620242932</v>
+        <v>0.0362618943639716</v>
       </c>
       <c r="C5">
-        <v>0.258814109740114</v>
+        <v>0.2589882165716723</v>
       </c>
       <c r="D5">
-        <v>0.8933527529779033</v>
+        <v>0.8933567801407576</v>
       </c>
       <c r="F5">
-        <v>0.144131099336961</v>
+        <v>0.1442170072470644</v>
       </c>
       <c r="G5">
-        <v>0.1134052076387853</v>
+        <v>0.1133672383287043</v>
       </c>
       <c r="H5">
-        <v>0.2797408209475182</v>
+        <v>0.2798484330095559</v>
       </c>
       <c r="I5">
-        <v>0.1162899990479887</v>
+        <v>0.1164079160348563</v>
       </c>
       <c r="J5">
-        <v>0.05119722944921867</v>
+        <v>0.05132365040150085</v>
       </c>
       <c r="K5">
-        <v>-0.1170648917985453</v>
+        <v>-0.117004729312769</v>
       </c>
       <c r="L5">
-        <v>-0.1641883656344368</v>
+        <v>-0.1641375756109109</v>
       </c>
       <c r="M5">
-        <v>0.1277166997456927</v>
+        <v>0.1277652650588194</v>
       </c>
       <c r="N5">
-        <v>0.124635290875092</v>
+        <v>0.124672080294903</v>
       </c>
       <c r="O5">
-        <v>0.2144706355428009</v>
+        <v>0.2144749012938966</v>
       </c>
       <c r="P5">
-        <v>0.5085842127016355</v>
+        <v>0.5086589493774576</v>
       </c>
       <c r="Q5">
-        <v>0.579497554608427</v>
+        <v>0.5794975316073759</v>
       </c>
       <c r="R5">
-        <v>-0.09204216806854483</v>
+        <v>-0.0918962480429867</v>
       </c>
       <c r="S5">
-        <v>-0.03227945394316144</v>
+        <v>-0.03210393587441602</v>
       </c>
       <c r="T5">
-        <v>0.5601751365216101</v>
+        <v>0.560202259159532</v>
       </c>
       <c r="U5">
         <v>-0.1116602514403753</v>
       </c>
       <c r="V5">
-        <v>0.2265620964953594</v>
+        <v>0.2266480702911372</v>
       </c>
       <c r="W5">
-        <v>0.3304971738961116</v>
+        <v>0.3305675279571635</v>
       </c>
       <c r="X5">
-        <v>0.5120956148953959</v>
+        <v>0.5122562333475724</v>
       </c>
       <c r="Y5">
-        <v>0.3745800475602408</v>
+        <v>0.3745608377052729</v>
       </c>
       <c r="Z5">
-        <v>0.5008625715029008</v>
+        <v>0.5008610353124552</v>
       </c>
       <c r="AA5">
-        <v>0.5167626951529453</v>
+        <v>0.5168002527260575</v>
       </c>
       <c r="AB5">
-        <v>0.4570231751505246</v>
+        <v>0.4570216054869827</v>
       </c>
     </row>
     <row r="6">
@@ -846,82 +846,82 @@
         </is>
       </c>
       <c r="B6">
-        <v>0.3356007386854665</v>
+        <v>0.3353035436244038</v>
       </c>
       <c r="C6">
-        <v>0.3034801346941386</v>
+        <v>0.3032054674842555</v>
       </c>
       <c r="D6">
-        <v>0.1100693107048966</v>
+        <v>0.1101013833874506</v>
       </c>
       <c r="E6">
-        <v>0.144131099336961</v>
+        <v>0.1442170072470644</v>
       </c>
       <c r="G6">
-        <v>0.3175308332936848</v>
+        <v>0.3177272721685255</v>
       </c>
       <c r="H6">
-        <v>-0.03577370495259154</v>
+        <v>-0.03510670429895189</v>
       </c>
       <c r="I6">
-        <v>0.3311037918510816</v>
+        <v>0.3308874443691532</v>
       </c>
       <c r="J6">
-        <v>0.3085845525873367</v>
+        <v>0.3083242242546798</v>
       </c>
       <c r="K6">
-        <v>0.1758125824951599</v>
+        <v>0.1755517833373934</v>
       </c>
       <c r="L6">
-        <v>0.1340896767583037</v>
+        <v>0.1337497712722012</v>
       </c>
       <c r="M6">
-        <v>0.09315039739234021</v>
+        <v>0.09301441959147191</v>
       </c>
       <c r="N6">
-        <v>0.08919686355013422</v>
+        <v>0.08909260643959102</v>
       </c>
       <c r="O6">
-        <v>0.05315059930657392</v>
+        <v>0.0531505027449837</v>
       </c>
       <c r="P6">
-        <v>0.2123556482429844</v>
+        <v>0.2122622921001213</v>
       </c>
       <c r="Q6">
-        <v>0.1735684875355147</v>
+        <v>0.1736201616372676</v>
       </c>
       <c r="R6">
-        <v>0.3057335380027029</v>
+        <v>0.3054321938811898</v>
       </c>
       <c r="S6">
-        <v>0.3266829287530781</v>
+        <v>0.326391697294726</v>
       </c>
       <c r="T6">
-        <v>0.1441448107370691</v>
+        <v>0.1441245155244848</v>
       </c>
       <c r="U6">
         <v>0.1574296744346301</v>
       </c>
       <c r="V6">
-        <v>0.01285106546278239</v>
+        <v>0.01263025020116457</v>
       </c>
       <c r="W6">
-        <v>0.07291304573384587</v>
+        <v>0.0727622101567849</v>
       </c>
       <c r="X6">
-        <v>0.3828874406165315</v>
+        <v>0.3827171378420469</v>
       </c>
       <c r="Y6">
-        <v>0.3584276905542873</v>
+        <v>0.3585951886045599</v>
       </c>
       <c r="Z6">
-        <v>0.4338956528085992</v>
+        <v>0.4339741721117608</v>
       </c>
       <c r="AA6">
-        <v>0.402214976646558</v>
+        <v>0.4021799804074211</v>
       </c>
       <c r="AB6">
-        <v>0.3257244311566102</v>
+        <v>0.3257884068861948</v>
       </c>
     </row>
     <row r="7">
@@ -931,82 +931,82 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.323111317324355</v>
+        <v>0.3236971878390013</v>
       </c>
       <c r="C7">
-        <v>0.3237570419414142</v>
+        <v>0.3239964682391911</v>
       </c>
       <c r="D7">
-        <v>0.06575060002858069</v>
+        <v>0.06573935776970632</v>
       </c>
       <c r="E7">
-        <v>0.1134052076387853</v>
+        <v>0.1133672383287043</v>
       </c>
       <c r="F7">
-        <v>0.3175308332936848</v>
+        <v>0.3177272721685255</v>
       </c>
       <c r="H7">
-        <v>0.02190532128656361</v>
+        <v>0.02149030032071721</v>
       </c>
       <c r="I7">
-        <v>0.282570268498868</v>
+        <v>0.2828530216981644</v>
       </c>
       <c r="J7">
-        <v>0.2636881031183485</v>
+        <v>0.2640401896402293</v>
       </c>
       <c r="K7">
-        <v>0.2611588492879401</v>
+        <v>0.2614278969556863</v>
       </c>
       <c r="L7">
-        <v>0.2601062661250715</v>
+        <v>0.2604577249577279</v>
       </c>
       <c r="M7">
-        <v>0.08503977019356276</v>
+        <v>0.08513926640104709</v>
       </c>
       <c r="N7">
-        <v>0.08038245758394995</v>
+        <v>0.08045849328625392</v>
       </c>
       <c r="O7">
-        <v>0.01816377007925208</v>
+        <v>0.01816571709808065</v>
       </c>
       <c r="P7">
-        <v>0.2185870666431455</v>
+        <v>0.218694363545172</v>
       </c>
       <c r="Q7">
-        <v>0.1062735002573635</v>
+        <v>0.1062571623805989</v>
       </c>
       <c r="R7">
-        <v>0.1707528146647875</v>
+        <v>0.1711986253962139</v>
       </c>
       <c r="S7">
-        <v>0.2100971853406813</v>
+        <v>0.2105637122323289</v>
       </c>
       <c r="T7">
-        <v>0.1201415305995272</v>
+        <v>0.1201756373706857</v>
       </c>
       <c r="U7">
         <v>0.1762047123370334</v>
       </c>
       <c r="V7">
-        <v>0.005446595930337673</v>
+        <v>0.005582451479098068</v>
       </c>
       <c r="W7">
-        <v>-0.1843850183102082</v>
+        <v>-0.184302951125371</v>
       </c>
       <c r="X7">
-        <v>0.42934677532029</v>
+        <v>0.4295964277789796</v>
       </c>
       <c r="Y7">
-        <v>0.7849799055840018</v>
+        <v>0.7849660069635523</v>
       </c>
       <c r="Z7">
-        <v>0.4859934247887432</v>
+        <v>0.4859926063769347</v>
       </c>
       <c r="AA7">
-        <v>0.4527763585237524</v>
+        <v>0.4528490542911307</v>
       </c>
       <c r="AB7">
-        <v>0.4851280844945142</v>
+        <v>0.4851276754370418</v>
       </c>
     </row>
     <row r="8">
@@ -1016,82 +1016,82 @@
         </is>
       </c>
       <c r="B8">
-        <v>-0.02416373461147085</v>
+        <v>-0.0225201660993329</v>
       </c>
       <c r="C8">
-        <v>0.050132066623324</v>
+        <v>0.05129771864827716</v>
       </c>
       <c r="D8">
-        <v>0.191491770102774</v>
+        <v>0.1916488558272403</v>
       </c>
       <c r="E8">
-        <v>0.2797408209475182</v>
+        <v>0.2798484330095559</v>
       </c>
       <c r="F8">
-        <v>-0.03577370495259154</v>
+        <v>-0.03510670429895189</v>
       </c>
       <c r="G8">
-        <v>0.02190532128656361</v>
+        <v>0.02149030032071721</v>
       </c>
       <c r="I8">
-        <v>-0.01989334939366471</v>
+        <v>-0.01892143169657567</v>
       </c>
       <c r="J8">
-        <v>-0.07623350148002871</v>
+        <v>-0.075132651862499</v>
       </c>
       <c r="K8">
-        <v>-0.1205504452645528</v>
+        <v>-0.1197490619453794</v>
       </c>
       <c r="L8">
-        <v>-0.1149895099678686</v>
+        <v>-0.113950251193763</v>
       </c>
       <c r="M8">
-        <v>-0.07855286707448961</v>
+        <v>-0.07818098883018644</v>
       </c>
       <c r="N8">
-        <v>-0.07656191525501457</v>
+        <v>-0.07628804370444969</v>
       </c>
       <c r="O8">
-        <v>0.01420358438361535</v>
+        <v>0.01424452783182506</v>
       </c>
       <c r="P8">
-        <v>0.275136092228879</v>
+        <v>0.275885638251716</v>
       </c>
       <c r="Q8">
-        <v>0.3498869658031392</v>
+        <v>0.3502217670037115</v>
       </c>
       <c r="R8">
-        <v>-0.1669674511727</v>
+        <v>-0.1656944313144815</v>
       </c>
       <c r="S8">
-        <v>-0.1293360697345566</v>
+        <v>-0.1279764998732663</v>
       </c>
       <c r="T8">
-        <v>0.3484443557673619</v>
+        <v>0.348997943631939</v>
       </c>
       <c r="U8">
         <v>-0.2131799171230018</v>
       </c>
       <c r="V8">
-        <v>0.05498920891964443</v>
+        <v>0.05571858693201029</v>
       </c>
       <c r="W8">
-        <v>0.03681155608437518</v>
+        <v>0.03734658138448063</v>
       </c>
       <c r="X8">
-        <v>0.1660969161404623</v>
+        <v>0.167118744581456</v>
       </c>
       <c r="Y8">
-        <v>0.1486366880162029</v>
+        <v>0.1484682200984068</v>
       </c>
       <c r="Z8">
-        <v>0.2109439578402317</v>
+        <v>0.2110968508457275</v>
       </c>
       <c r="AA8">
-        <v>0.1606220018697473</v>
+        <v>0.1610634092400903</v>
       </c>
       <c r="AB8">
-        <v>0.09535162847028097</v>
+        <v>0.09538601469481374</v>
       </c>
     </row>
     <row r="9">
@@ -1101,82 +1101,82 @@
         </is>
       </c>
       <c r="B9">
-        <v>0.8961955493199838</v>
+        <v>0.8962132468714507</v>
       </c>
       <c r="C9">
-        <v>0.2555038889054406</v>
+        <v>0.2550760362606682</v>
       </c>
       <c r="D9">
-        <v>0.2257039874244228</v>
+        <v>0.2257782358420033</v>
       </c>
       <c r="E9">
-        <v>0.1162899990479887</v>
+        <v>0.1164079160348563</v>
       </c>
       <c r="F9">
-        <v>0.3311037918510816</v>
+        <v>0.3308874443691532</v>
       </c>
       <c r="G9">
-        <v>0.282570268498868</v>
+        <v>0.2828530216981644</v>
       </c>
       <c r="H9">
-        <v>-0.01989334939366471</v>
+        <v>-0.01892143169657567</v>
       </c>
       <c r="J9">
-        <v>0.9712439260222197</v>
+        <v>0.9712376187738408</v>
       </c>
       <c r="K9">
-        <v>0.4381476825804904</v>
+        <v>0.4378938308009257</v>
       </c>
       <c r="L9">
-        <v>0.4196530061222157</v>
+        <v>0.419327418664915</v>
       </c>
       <c r="M9">
-        <v>0.4312321614359071</v>
+        <v>0.4311387230466044</v>
       </c>
       <c r="N9">
-        <v>0.4222198254083336</v>
+        <v>0.4221636708752149</v>
       </c>
       <c r="O9">
-        <v>0.07873934663441608</v>
+        <v>0.07874567696688811</v>
       </c>
       <c r="P9">
-        <v>0.2569300336759371</v>
+        <v>0.2568221946204033</v>
       </c>
       <c r="Q9">
-        <v>0.09747366529779616</v>
+        <v>0.09753912176323662</v>
       </c>
       <c r="R9">
-        <v>0.1913496921202967</v>
+        <v>0.1908115306086125</v>
       </c>
       <c r="S9">
-        <v>0.1745658559269074</v>
+        <v>0.1740021193325153</v>
       </c>
       <c r="T9">
-        <v>0.07221838687108741</v>
+        <v>0.07218036953787371</v>
       </c>
       <c r="U9">
         <v>0.2773549624024398</v>
       </c>
       <c r="V9">
-        <v>0.2126854678990742</v>
+        <v>0.2124414934558372</v>
       </c>
       <c r="W9">
-        <v>0.2292670244879615</v>
+        <v>0.2291028197658982</v>
       </c>
       <c r="X9">
-        <v>0.4206130835491929</v>
+        <v>0.4203893727952895</v>
       </c>
       <c r="Y9">
-        <v>0.3991283453381945</v>
+        <v>0.3993910979703796</v>
       </c>
       <c r="Z9">
-        <v>0.4547064339983174</v>
+        <v>0.4548509819244133</v>
       </c>
       <c r="AA9">
-        <v>0.4403194251699888</v>
+        <v>0.4403050500102345</v>
       </c>
       <c r="AB9">
-        <v>0.4608884507285015</v>
+        <v>0.4610309462425894</v>
       </c>
     </row>
     <row r="10">
@@ -1186,82 +1186,82 @@
         </is>
       </c>
       <c r="B10">
-        <v>0.8869678248564653</v>
+        <v>0.8869066548957314</v>
       </c>
       <c r="C10">
-        <v>0.2360206752074876</v>
+        <v>0.2355100635389874</v>
       </c>
       <c r="D10">
-        <v>0.1694901819227861</v>
+        <v>0.1695741123063069</v>
       </c>
       <c r="E10">
-        <v>0.05119722944921867</v>
+        <v>0.05132365040150085</v>
       </c>
       <c r="F10">
-        <v>0.3085845525873367</v>
+        <v>0.3083242242546798</v>
       </c>
       <c r="G10">
-        <v>0.2636881031183485</v>
+        <v>0.2640401896402293</v>
       </c>
       <c r="H10">
-        <v>-0.07623350148002871</v>
+        <v>-0.075132651862499</v>
       </c>
       <c r="I10">
-        <v>0.9712439260222197</v>
+        <v>0.9712376187738408</v>
       </c>
       <c r="K10">
-        <v>0.4554010135828829</v>
+        <v>0.4551094903349868</v>
       </c>
       <c r="L10">
-        <v>0.4375390915858224</v>
+        <v>0.4371521233224544</v>
       </c>
       <c r="M10">
-        <v>0.4157042652448103</v>
+        <v>0.4156064554248929</v>
       </c>
       <c r="N10">
-        <v>0.4077589653316137</v>
+        <v>0.4077082805258652</v>
       </c>
       <c r="O10">
-        <v>0.05670937951115437</v>
+        <v>0.05671414325509426</v>
       </c>
       <c r="P10">
-        <v>0.2008570865655303</v>
+        <v>0.2007180287572574</v>
       </c>
       <c r="Q10">
-        <v>0.02912609774579458</v>
+        <v>0.02918843718686302</v>
       </c>
       <c r="R10">
-        <v>0.2125823878659584</v>
+        <v>0.2119291190826943</v>
       </c>
       <c r="S10">
-        <v>0.1845657401655993</v>
+        <v>0.1838740132833975</v>
       </c>
       <c r="T10">
-        <v>0.009530944535091615</v>
+        <v>0.009466718180983732</v>
       </c>
       <c r="U10">
         <v>0.2944477371716243</v>
       </c>
       <c r="V10">
-        <v>0.1903735066941332</v>
+        <v>0.1900765496726321</v>
       </c>
       <c r="W10">
-        <v>0.2149581194945659</v>
+        <v>0.2147644491992538</v>
       </c>
       <c r="X10">
-        <v>0.3722160446906417</v>
+        <v>0.3719322857189268</v>
       </c>
       <c r="Y10">
-        <v>0.3642934523720785</v>
+        <v>0.3646221304709235</v>
       </c>
       <c r="Z10">
-        <v>0.4033906328573477</v>
+        <v>0.4035747326591186</v>
       </c>
       <c r="AA10">
-        <v>0.391116051336554</v>
+        <v>0.3911057785114367</v>
       </c>
       <c r="AB10">
-        <v>0.4249354903462267</v>
+        <v>0.4251231670392321</v>
       </c>
     </row>
     <row r="11">
@@ -1271,82 +1271,82 @@
         </is>
       </c>
       <c r="B11">
-        <v>0.4924517349744275</v>
+        <v>0.4921262584614316</v>
       </c>
       <c r="C11">
-        <v>0.142226497343822</v>
+        <v>0.1417578490238693</v>
       </c>
       <c r="D11">
-        <v>-0.01993059353965762</v>
+        <v>-0.01991398570375038</v>
       </c>
       <c r="E11">
-        <v>-0.1170648917985453</v>
+        <v>-0.117004729312769</v>
       </c>
       <c r="F11">
-        <v>0.1758125824951599</v>
+        <v>0.1755517833373934</v>
       </c>
       <c r="G11">
-        <v>0.2611588492879401</v>
+        <v>0.2614278969556863</v>
       </c>
       <c r="H11">
-        <v>-0.1205504452645528</v>
+        <v>-0.1197490619453794</v>
       </c>
       <c r="I11">
-        <v>0.4381476825804904</v>
+        <v>0.4378938308009257</v>
       </c>
       <c r="J11">
-        <v>0.4554010135828829</v>
+        <v>0.4551094903349868</v>
       </c>
       <c r="L11">
-        <v>0.8963277253782602</v>
+        <v>0.8962841935867969</v>
       </c>
       <c r="M11">
-        <v>0.1867578797682257</v>
+        <v>0.186601532271996</v>
       </c>
       <c r="N11">
-        <v>0.1928430072542302</v>
+        <v>0.1927308280386089</v>
       </c>
       <c r="O11">
-        <v>0.05124331053679738</v>
+        <v>0.05124348000204136</v>
       </c>
       <c r="P11">
-        <v>0.09984627655841705</v>
+        <v>0.09969716055863168</v>
       </c>
       <c r="Q11">
-        <v>-0.0454330206277398</v>
+        <v>-0.04540124905632316</v>
       </c>
       <c r="R11">
-        <v>0.1490431290543824</v>
+        <v>0.1484653638711309</v>
       </c>
       <c r="S11">
-        <v>0.1425395885098989</v>
+        <v>0.1419493414715042</v>
       </c>
       <c r="T11">
-        <v>-0.06082283478817578</v>
+        <v>-0.06089198647750246</v>
       </c>
       <c r="U11">
         <v>0.218405064445904</v>
       </c>
       <c r="V11">
-        <v>0.114768702086555</v>
+        <v>0.1145027921456115</v>
       </c>
       <c r="W11">
-        <v>0.01585083925799619</v>
+        <v>0.01563150988028812</v>
       </c>
       <c r="X11">
-        <v>0.1358318361040546</v>
+        <v>0.1355090426346558</v>
       </c>
       <c r="Y11">
-        <v>0.2630782637138436</v>
+        <v>0.263296988813303</v>
       </c>
       <c r="Z11">
-        <v>0.1426450415060509</v>
+        <v>0.142712643179018</v>
       </c>
       <c r="AA11">
-        <v>0.1651244743268797</v>
+        <v>0.1650434677702124</v>
       </c>
       <c r="AB11">
-        <v>0.2128236763995898</v>
+        <v>0.2129034349415712</v>
       </c>
     </row>
     <row r="12">
@@ -1356,82 +1356,82 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.4806230822728826</v>
+        <v>0.4801512826445933</v>
       </c>
       <c r="C12">
-        <v>0.1382328154541606</v>
+        <v>0.1376612696948288</v>
       </c>
       <c r="D12">
-        <v>-0.05656662657225147</v>
+        <v>-0.0565600227370593</v>
       </c>
       <c r="E12">
-        <v>-0.1641883656344368</v>
+        <v>-0.1641375756109109</v>
       </c>
       <c r="F12">
-        <v>0.1340896767583037</v>
+        <v>0.1337497712722012</v>
       </c>
       <c r="G12">
-        <v>0.2601062661250715</v>
+        <v>0.2604577249577279</v>
       </c>
       <c r="H12">
-        <v>-0.1149895099678686</v>
+        <v>-0.113950251193763</v>
       </c>
       <c r="I12">
-        <v>0.4196530061222157</v>
+        <v>0.419327418664915</v>
       </c>
       <c r="J12">
-        <v>0.4375390915858224</v>
+        <v>0.4371521233224544</v>
       </c>
       <c r="K12">
-        <v>0.8963277253782602</v>
+        <v>0.8962841935867969</v>
       </c>
       <c r="M12">
-        <v>0.1816156914328293</v>
+        <v>0.1814265173404312</v>
       </c>
       <c r="N12">
-        <v>0.1874068278411156</v>
+        <v>0.1872742694289936</v>
       </c>
       <c r="O12">
-        <v>0.04923039928983854</v>
+        <v>0.04923288234022009</v>
       </c>
       <c r="P12">
-        <v>0.1043686881558954</v>
+        <v>0.1041883253381078</v>
       </c>
       <c r="Q12">
-        <v>-0.07518607764377164</v>
+        <v>-0.07516055710950412</v>
       </c>
       <c r="R12">
-        <v>0.1199256999386818</v>
+        <v>0.1191647463280724</v>
       </c>
       <c r="S12">
-        <v>0.1114668340092859</v>
+        <v>0.110689173661287</v>
       </c>
       <c r="T12">
-        <v>-0.04960957447168565</v>
+        <v>-0.04969761963597166</v>
       </c>
       <c r="U12">
         <v>0.22227748487964</v>
       </c>
       <c r="V12">
-        <v>0.1172696897046826</v>
+        <v>0.1169420100048394</v>
       </c>
       <c r="W12">
-        <v>-0.002920971674548827</v>
+        <v>-0.003203787163278293</v>
       </c>
       <c r="X12">
-        <v>0.1063476770020601</v>
+        <v>0.105931356113506</v>
       </c>
       <c r="Y12">
-        <v>0.2423586880872797</v>
+        <v>0.2426416938901234</v>
       </c>
       <c r="Z12">
-        <v>0.09467593427367921</v>
+        <v>0.09475061337807365</v>
       </c>
       <c r="AA12">
-        <v>0.1418886941619668</v>
+        <v>0.1417871818067766</v>
       </c>
       <c r="AB12">
-        <v>0.1844911853384518</v>
+        <v>0.1845936274901514</v>
       </c>
     </row>
     <row r="13">
@@ -1441,82 +1441,82 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.4215582337954846</v>
+        <v>0.421497118288005</v>
       </c>
       <c r="C13">
-        <v>0.1205740240577348</v>
+        <v>0.1203247618736048</v>
       </c>
       <c r="D13">
-        <v>0.2952329416539339</v>
+        <v>0.2952574023671488</v>
       </c>
       <c r="E13">
-        <v>0.1277166997456927</v>
+        <v>0.1277652650588194</v>
       </c>
       <c r="F13">
-        <v>0.09315039739234021</v>
+        <v>0.09301441959147191</v>
       </c>
       <c r="G13">
-        <v>0.08503977019356276</v>
+        <v>0.08513926640104709</v>
       </c>
       <c r="H13">
-        <v>-0.07855286707448961</v>
+        <v>-0.07818098883018644</v>
       </c>
       <c r="I13">
-        <v>0.4312321614359071</v>
+        <v>0.4311387230466044</v>
       </c>
       <c r="J13">
-        <v>0.4157042652448103</v>
+        <v>0.4156064554248929</v>
       </c>
       <c r="K13">
-        <v>0.1867578797682257</v>
+        <v>0.186601532271996</v>
       </c>
       <c r="L13">
-        <v>0.1816156914328293</v>
+        <v>0.1814265173404312</v>
       </c>
       <c r="N13">
-        <v>0.9930582940454148</v>
+        <v>0.9930601937599935</v>
       </c>
       <c r="O13">
-        <v>0.4814260444483036</v>
+        <v>0.4814443693986965</v>
       </c>
       <c r="P13">
-        <v>0.4982513699967038</v>
+        <v>0.4982138529267472</v>
       </c>
       <c r="Q13">
-        <v>0.1192524376357505</v>
+        <v>0.1192758446805697</v>
       </c>
       <c r="R13">
-        <v>-0.03410757452773534</v>
+        <v>-0.03441708348787718</v>
       </c>
       <c r="S13">
-        <v>-0.03472590134892537</v>
+        <v>-0.03504207961216314</v>
       </c>
       <c r="T13">
-        <v>0.150279374245199</v>
+        <v>0.1502627708979039</v>
       </c>
       <c r="U13">
         <v>0.09167169792894313</v>
       </c>
       <c r="V13">
-        <v>0.2309812695323909</v>
+        <v>0.2308717480747141</v>
       </c>
       <c r="W13">
-        <v>0.2110854864861658</v>
+        <v>0.2110039610517267</v>
       </c>
       <c r="X13">
-        <v>0.2390575036400336</v>
+        <v>0.2389280818470994</v>
       </c>
       <c r="Y13">
-        <v>0.2097341033105758</v>
+        <v>0.2098212833323626</v>
       </c>
       <c r="Z13">
-        <v>0.2170902074544813</v>
+        <v>0.2171166148616001</v>
       </c>
       <c r="AA13">
-        <v>0.2634668864320083</v>
+        <v>0.2634258936300762</v>
       </c>
       <c r="AB13">
-        <v>0.2561259642933945</v>
+        <v>0.2561537760680311</v>
       </c>
     </row>
     <row r="14">
@@ -1526,82 +1526,82 @@
         </is>
       </c>
       <c r="B14">
-        <v>0.4135082113170079</v>
+        <v>0.4135145171964408</v>
       </c>
       <c r="C14">
-        <v>0.1215203709956318</v>
+        <v>0.1213179227496275</v>
       </c>
       <c r="D14">
-        <v>0.2902142175037654</v>
+        <v>0.2902305768007128</v>
       </c>
       <c r="E14">
-        <v>0.124635290875092</v>
+        <v>0.124672080294903</v>
       </c>
       <c r="F14">
-        <v>0.08919686355013422</v>
+        <v>0.08909260643959102</v>
       </c>
       <c r="G14">
-        <v>0.08038245758394995</v>
+        <v>0.08045849328625392</v>
       </c>
       <c r="H14">
-        <v>-0.07656191525501457</v>
+        <v>-0.07628804370444969</v>
       </c>
       <c r="I14">
-        <v>0.4222198254083336</v>
+        <v>0.4221636708752149</v>
       </c>
       <c r="J14">
-        <v>0.4077589653316137</v>
+        <v>0.4077082805258652</v>
       </c>
       <c r="K14">
-        <v>0.1928430072542302</v>
+        <v>0.1927308280386089</v>
       </c>
       <c r="L14">
-        <v>0.1874068278411156</v>
+        <v>0.1872742694289936</v>
       </c>
       <c r="M14">
-        <v>0.9930582940454148</v>
+        <v>0.9930601937599935</v>
       </c>
       <c r="O14">
-        <v>0.4867127789044392</v>
+        <v>0.4867230732292473</v>
       </c>
       <c r="P14">
-        <v>0.5073781878161772</v>
+        <v>0.5073508488973718</v>
       </c>
       <c r="Q14">
-        <v>0.1189627596697698</v>
+        <v>0.1189792709547957</v>
       </c>
       <c r="R14">
-        <v>-0.04148637770958501</v>
+        <v>-0.04172526642003677</v>
       </c>
       <c r="S14">
-        <v>-0.03993055744401103</v>
+        <v>-0.04017403757573355</v>
       </c>
       <c r="T14">
-        <v>0.1536935129337068</v>
+        <v>0.153680112528515</v>
       </c>
       <c r="U14">
         <v>0.08802685745852554</v>
       </c>
       <c r="V14">
-        <v>0.2314956670707393</v>
+        <v>0.2314141110879342</v>
       </c>
       <c r="W14">
-        <v>0.208477323077658</v>
+        <v>0.2084157308403661</v>
       </c>
       <c r="X14">
-        <v>0.2345165124716445</v>
+        <v>0.2344215023238028</v>
       </c>
       <c r="Y14">
-        <v>0.2063373161092445</v>
+        <v>0.2064034817014902</v>
       </c>
       <c r="Z14">
-        <v>0.2095966809277022</v>
+        <v>0.2096149304223076</v>
       </c>
       <c r="AA14">
-        <v>0.2596212709662951</v>
+        <v>0.2595878516039381</v>
       </c>
       <c r="AB14">
-        <v>0.2472411800837875</v>
+        <v>0.2472603294569372</v>
       </c>
     </row>
     <row r="15">
@@ -1611,82 +1611,82 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.0471792537068802</v>
+        <v>0.04719042423220197</v>
       </c>
       <c r="C15">
-        <v>0.07245568199727372</v>
+        <v>0.07244794954821077</v>
       </c>
       <c r="D15">
-        <v>0.283556000835911</v>
+        <v>0.2835567453757912</v>
       </c>
       <c r="E15">
-        <v>0.2144706355428009</v>
+        <v>0.2144749012938966</v>
       </c>
       <c r="F15">
-        <v>0.05315059930657392</v>
+        <v>0.0531505027449837</v>
       </c>
       <c r="G15">
-        <v>0.01816377007925208</v>
+        <v>0.01816571709808065</v>
       </c>
       <c r="H15">
-        <v>0.01420358438361535</v>
+        <v>0.01424452783182506</v>
       </c>
       <c r="I15">
-        <v>0.07873934663441608</v>
+        <v>0.07874567696688811</v>
       </c>
       <c r="J15">
-        <v>0.05670937951115437</v>
+        <v>0.05671414325509426</v>
       </c>
       <c r="K15">
-        <v>0.05124331053679738</v>
+        <v>0.05124348000204136</v>
       </c>
       <c r="L15">
-        <v>0.04923039928983854</v>
+        <v>0.04923288234022009</v>
       </c>
       <c r="M15">
-        <v>0.4814260444483036</v>
+        <v>0.4814443693986965</v>
       </c>
       <c r="N15">
-        <v>0.4867127789044392</v>
+        <v>0.4867230732292473</v>
       </c>
       <c r="P15">
-        <v>0.3751373556618486</v>
+        <v>0.3751519894817744</v>
       </c>
       <c r="Q15">
-        <v>0.2270251724431761</v>
+        <v>0.2270249835937784</v>
       </c>
       <c r="R15">
-        <v>-0.1576237293557037</v>
+        <v>-0.1576871134965886</v>
       </c>
       <c r="S15">
-        <v>-0.1149317661250067</v>
+        <v>-0.1149810790924108</v>
       </c>
       <c r="T15">
-        <v>0.255725069652889</v>
+        <v>0.2557265663160282</v>
       </c>
       <c r="U15">
         <v>-0.1173516718667757</v>
       </c>
       <c r="V15">
-        <v>0.1143778684184701</v>
+        <v>0.1143822773826612</v>
       </c>
       <c r="W15">
-        <v>0.02419352604874877</v>
+        <v>0.02419368910670603</v>
       </c>
       <c r="X15">
-        <v>0.06806584446781606</v>
+        <v>0.06806721577069377</v>
       </c>
       <c r="Y15">
-        <v>0.07022914083834858</v>
+        <v>0.07023256420821834</v>
       </c>
       <c r="Z15">
-        <v>0.03739113956807818</v>
+        <v>0.03739180388502106</v>
       </c>
       <c r="AA15">
-        <v>0.08981717284198396</v>
+        <v>0.08981542741864301</v>
       </c>
       <c r="AB15">
-        <v>0.06216503371454456</v>
+        <v>0.06216594163126758</v>
       </c>
     </row>
     <row r="16">
@@ -1696,82 +1696,82 @@
         </is>
       </c>
       <c r="B16">
-        <v>0.2278437120825874</v>
+        <v>0.2277054854577264</v>
       </c>
       <c r="C16">
-        <v>0.3012398029380268</v>
+        <v>0.3011142612197973</v>
       </c>
       <c r="D16">
-        <v>0.5460714273553775</v>
+        <v>0.5461144914187797</v>
       </c>
       <c r="E16">
-        <v>0.5085842127016355</v>
+        <v>0.5086589493774576</v>
       </c>
       <c r="F16">
-        <v>0.2123556482429844</v>
+        <v>0.2122622921001213</v>
       </c>
       <c r="G16">
-        <v>0.2185870666431455</v>
+        <v>0.218694363545172</v>
       </c>
       <c r="H16">
-        <v>0.275136092228879</v>
+        <v>0.275885638251716</v>
       </c>
       <c r="I16">
-        <v>0.2569300336759371</v>
+        <v>0.2568221946204033</v>
       </c>
       <c r="J16">
-        <v>0.2008570865655303</v>
+        <v>0.2007180287572574</v>
       </c>
       <c r="K16">
-        <v>0.09984627655841705</v>
+        <v>0.09969716055863168</v>
       </c>
       <c r="L16">
-        <v>0.1043686881558954</v>
+        <v>0.1041883253381078</v>
       </c>
       <c r="M16">
-        <v>0.4982513699967038</v>
+        <v>0.4982138529267472</v>
       </c>
       <c r="N16">
-        <v>0.5073781878161772</v>
+        <v>0.5073508488973718</v>
       </c>
       <c r="O16">
-        <v>0.3751373556618486</v>
+        <v>0.3751519894817744</v>
       </c>
       <c r="Q16">
-        <v>0.8019980528289139</v>
+        <v>0.8020419371435977</v>
       </c>
       <c r="R16">
-        <v>-0.1011757669094605</v>
+        <v>-0.1014788246072017</v>
       </c>
       <c r="S16">
-        <v>-0.03587327219940296</v>
+        <v>-0.03615342245176581</v>
       </c>
       <c r="T16">
-        <v>0.8641202561226123</v>
+        <v>0.8641310656617663</v>
       </c>
       <c r="U16">
         <v>-0.08868916681725575</v>
       </c>
       <c r="V16">
-        <v>0.1974318804169292</v>
+        <v>0.1973406508596656</v>
       </c>
       <c r="W16">
-        <v>0.2070815185909677</v>
+        <v>0.2070137007676557</v>
       </c>
       <c r="X16">
-        <v>0.4027671987637017</v>
+        <v>0.4026988190641543</v>
       </c>
       <c r="Y16">
-        <v>0.429196151826006</v>
+        <v>0.4293052952424644</v>
       </c>
       <c r="Z16">
-        <v>0.3866910709182386</v>
+        <v>0.3867402416113038</v>
       </c>
       <c r="AA16">
-        <v>0.4368691245825451</v>
+        <v>0.4368541251507124</v>
       </c>
       <c r="AB16">
-        <v>0.3723253045936368</v>
+        <v>0.3723707059350114</v>
       </c>
     </row>
     <row r="17">
@@ -1781,82 +1781,82 @@
         </is>
       </c>
       <c r="B17">
-        <v>0.04392118386067694</v>
+        <v>0.04402615507213722</v>
       </c>
       <c r="C17">
-        <v>0.2372756646158307</v>
+        <v>0.2373910808748982</v>
       </c>
       <c r="D17">
-        <v>0.5304481930814725</v>
+        <v>0.5304458016652085</v>
       </c>
       <c r="E17">
-        <v>0.579497554608427</v>
+        <v>0.5794975316073759</v>
       </c>
       <c r="F17">
-        <v>0.1735684875355147</v>
+        <v>0.1736201616372676</v>
       </c>
       <c r="G17">
-        <v>0.1062735002573635</v>
+        <v>0.1062571623805989</v>
       </c>
       <c r="H17">
-        <v>0.3498869658031392</v>
+        <v>0.3502217670037115</v>
       </c>
       <c r="I17">
-        <v>0.09747366529779616</v>
+        <v>0.09753912176323662</v>
       </c>
       <c r="J17">
-        <v>0.02912609774579458</v>
+        <v>0.02918843718686302</v>
       </c>
       <c r="K17">
-        <v>-0.0454330206277398</v>
+        <v>-0.04540124905632316</v>
       </c>
       <c r="L17">
-        <v>-0.07518607764377164</v>
+        <v>-0.07516055710950412</v>
       </c>
       <c r="M17">
-        <v>0.1192524376357505</v>
+        <v>0.1192758446805697</v>
       </c>
       <c r="N17">
-        <v>0.1189627596697698</v>
+        <v>0.1189792709547957</v>
       </c>
       <c r="O17">
-        <v>0.2270251724431761</v>
+        <v>0.2270249835937784</v>
       </c>
       <c r="P17">
-        <v>0.8019980528289139</v>
+        <v>0.8020419371435977</v>
       </c>
       <c r="R17">
-        <v>-0.143428641645877</v>
+        <v>-0.143430232537778</v>
       </c>
       <c r="S17">
-        <v>-0.07786492792613323</v>
+        <v>-0.0778411579523758</v>
       </c>
       <c r="T17">
-        <v>0.9466157878052852</v>
+        <v>0.9466253699514651</v>
       </c>
       <c r="U17">
         <v>-0.1799687160309316</v>
       </c>
       <c r="V17">
-        <v>0.10683661479572</v>
+        <v>0.1068761516923098</v>
       </c>
       <c r="W17">
-        <v>0.1572623816922726</v>
+        <v>0.1572928563188545</v>
       </c>
       <c r="X17">
-        <v>0.3028107849434409</v>
+        <v>0.3028899548277057</v>
       </c>
       <c r="Y17">
-        <v>0.2913049507773651</v>
+        <v>0.2912993446265165</v>
       </c>
       <c r="Z17">
-        <v>0.3211566183355837</v>
+        <v>0.321152607530685</v>
       </c>
       <c r="AA17">
-        <v>0.3171446190060881</v>
+        <v>0.3171560124960915</v>
       </c>
       <c r="AB17">
-        <v>0.248237768223168</v>
+        <v>0.2482325913431211</v>
       </c>
     </row>
     <row r="18">
@@ -1866,82 +1866,82 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.2223037733492779</v>
+        <v>0.2213858907085259</v>
       </c>
       <c r="C18">
-        <v>0.1712511148831177</v>
+        <v>0.1706431063113516</v>
       </c>
       <c r="D18">
-        <v>-0.1240975527565239</v>
+        <v>-0.1240677449488455</v>
       </c>
       <c r="E18">
-        <v>-0.09204216806854483</v>
+        <v>-0.0918962480429867</v>
       </c>
       <c r="F18">
-        <v>0.3057335380027029</v>
+        <v>0.3054321938811898</v>
       </c>
       <c r="G18">
-        <v>0.1707528146647875</v>
+        <v>0.1711986253962139</v>
       </c>
       <c r="H18">
-        <v>-0.1669674511727</v>
+        <v>-0.1656944313144815</v>
       </c>
       <c r="I18">
-        <v>0.1913496921202967</v>
+        <v>0.1908115306086125</v>
       </c>
       <c r="J18">
-        <v>0.2125823878659584</v>
+        <v>0.2119291190826943</v>
       </c>
       <c r="K18">
-        <v>0.1490431290543824</v>
+        <v>0.1484653638711309</v>
       </c>
       <c r="L18">
-        <v>0.1199256999386818</v>
+        <v>0.1191647463280724</v>
       </c>
       <c r="M18">
-        <v>-0.03410757452773534</v>
+        <v>-0.03441708348787718</v>
       </c>
       <c r="N18">
-        <v>-0.04148637770958501</v>
+        <v>-0.04172526642003677</v>
       </c>
       <c r="O18">
-        <v>-0.1576237293557037</v>
+        <v>-0.1576871134965886</v>
       </c>
       <c r="P18">
-        <v>-0.1011757669094605</v>
+        <v>-0.1014788246072017</v>
       </c>
       <c r="Q18">
-        <v>-0.143428641645877</v>
+        <v>-0.143430232537778</v>
       </c>
       <c r="S18">
-        <v>0.961359379722571</v>
+        <v>0.9613207253471929</v>
       </c>
       <c r="T18">
-        <v>-0.169301033683831</v>
+        <v>-0.1694610076243347</v>
       </c>
       <c r="U18">
         <v>0.3184190306397158</v>
       </c>
       <c r="V18">
-        <v>-0.07828055500257634</v>
+        <v>-0.07880303477807618</v>
       </c>
       <c r="W18">
-        <v>0.1457812084915509</v>
+        <v>0.1455198349663011</v>
       </c>
       <c r="X18">
-        <v>0.2550128996497166</v>
+        <v>0.2546362214002177</v>
       </c>
       <c r="Y18">
-        <v>0.1761153044475365</v>
+        <v>0.1765187466263051</v>
       </c>
       <c r="Z18">
-        <v>0.301855794251151</v>
+        <v>0.3021549368649482</v>
       </c>
       <c r="AA18">
-        <v>0.2707777589529218</v>
+        <v>0.2708006212946851</v>
       </c>
       <c r="AB18">
-        <v>0.253816369114977</v>
+        <v>0.2540893277464856</v>
       </c>
     </row>
     <row r="19">
@@ -1951,82 +1951,82 @@
         </is>
       </c>
       <c r="B19">
-        <v>0.2051755593973502</v>
+        <v>0.2042195690993944</v>
       </c>
       <c r="C19">
-        <v>0.1975531061210007</v>
+        <v>0.196962808104921</v>
       </c>
       <c r="D19">
-        <v>-0.07447256535857966</v>
+        <v>-0.07442091165502744</v>
       </c>
       <c r="E19">
-        <v>-0.03227945394316144</v>
+        <v>-0.03210393587441602</v>
       </c>
       <c r="F19">
-        <v>0.3266829287530781</v>
+        <v>0.326391697294726</v>
       </c>
       <c r="G19">
-        <v>0.2100971853406813</v>
+        <v>0.2105637122323289</v>
       </c>
       <c r="H19">
-        <v>-0.1293360697345566</v>
+        <v>-0.1279764998732663</v>
       </c>
       <c r="I19">
-        <v>0.1745658559269074</v>
+        <v>0.1740021193325153</v>
       </c>
       <c r="J19">
-        <v>0.1845657401655993</v>
+        <v>0.1838740132833975</v>
       </c>
       <c r="K19">
-        <v>0.1425395885098989</v>
+        <v>0.1419493414715042</v>
       </c>
       <c r="L19">
-        <v>0.1114668340092859</v>
+        <v>0.110689173661287</v>
       </c>
       <c r="M19">
-        <v>-0.03472590134892537</v>
+        <v>-0.03504207961216314</v>
       </c>
       <c r="N19">
-        <v>-0.03993055744401103</v>
+        <v>-0.04017403757573355</v>
       </c>
       <c r="O19">
-        <v>-0.1149317661250067</v>
+        <v>-0.1149810790924108</v>
       </c>
       <c r="P19">
-        <v>-0.03587327219940296</v>
+        <v>-0.03615342245176581</v>
       </c>
       <c r="Q19">
-        <v>-0.07786492792613323</v>
+        <v>-0.0778411579523758</v>
       </c>
       <c r="R19">
-        <v>0.961359379722571</v>
+        <v>0.9613207253471929</v>
       </c>
       <c r="T19">
-        <v>-0.09765281689795575</v>
+        <v>-0.09778530775868367</v>
       </c>
       <c r="U19">
         <v>0.267252901115227</v>
       </c>
       <c r="V19">
-        <v>-0.09232738737452428</v>
+        <v>-0.0928560701431425</v>
       </c>
       <c r="W19">
-        <v>0.1209896636107201</v>
+        <v>0.1207163207946081</v>
       </c>
       <c r="X19">
-        <v>0.2814961750712565</v>
+        <v>0.2811295216726082</v>
       </c>
       <c r="Y19">
-        <v>0.2228714859878356</v>
+        <v>0.2232979146494285</v>
       </c>
       <c r="Z19">
-        <v>0.3350302487284268</v>
+        <v>0.3353452951229174</v>
       </c>
       <c r="AA19">
-        <v>0.3013835204144575</v>
+        <v>0.301417717964827</v>
       </c>
       <c r="AB19">
-        <v>0.2812811894268327</v>
+        <v>0.2815588767505635</v>
       </c>
     </row>
     <row r="20">
@@ -2036,82 +2036,82 @@
         </is>
       </c>
       <c r="B20">
-        <v>0.02379716288421419</v>
+        <v>0.02371808510163974</v>
       </c>
       <c r="C20">
-        <v>0.2325718912451744</v>
+        <v>0.2325793648313662</v>
       </c>
       <c r="D20">
-        <v>0.5423124177789915</v>
+        <v>0.5423234575359206</v>
       </c>
       <c r="E20">
-        <v>0.5601751365216101</v>
+        <v>0.560202259159532</v>
       </c>
       <c r="F20">
-        <v>0.1441448107370691</v>
+        <v>0.1441245155244848</v>
       </c>
       <c r="G20">
-        <v>0.1201415305995272</v>
+        <v>0.1201756373706857</v>
       </c>
       <c r="H20">
-        <v>0.3484443557673619</v>
+        <v>0.348997943631939</v>
       </c>
       <c r="I20">
-        <v>0.07221838687108741</v>
+        <v>0.07218036953787371</v>
       </c>
       <c r="J20">
-        <v>0.009530944535091615</v>
+        <v>0.009466718180983732</v>
       </c>
       <c r="K20">
-        <v>-0.06082283478817578</v>
+        <v>-0.06089198647750246</v>
       </c>
       <c r="L20">
-        <v>-0.04960957447168565</v>
+        <v>-0.04969761963597166</v>
       </c>
       <c r="M20">
-        <v>0.150279374245199</v>
+        <v>0.1502627708979039</v>
       </c>
       <c r="N20">
-        <v>0.1536935129337068</v>
+        <v>0.153680112528515</v>
       </c>
       <c r="O20">
-        <v>0.255725069652889</v>
+        <v>0.2557265663160282</v>
       </c>
       <c r="P20">
-        <v>0.8641202561226123</v>
+        <v>0.8641310656617663</v>
       </c>
       <c r="Q20">
-        <v>0.9466157878052852</v>
+        <v>0.9466253699514651</v>
       </c>
       <c r="R20">
-        <v>-0.169301033683831</v>
+        <v>-0.1694610076243347</v>
       </c>
       <c r="S20">
-        <v>-0.09765281689795575</v>
+        <v>-0.09778530775868367</v>
       </c>
       <c r="U20">
         <v>-0.2198006607497221</v>
       </c>
       <c r="V20">
-        <v>0.1261760819536201</v>
+        <v>0.1261521508710033</v>
       </c>
       <c r="W20">
-        <v>0.1515094285417939</v>
+        <v>0.1514918092120514</v>
       </c>
       <c r="X20">
-        <v>0.291850726205502</v>
+        <v>0.2918502019583458</v>
       </c>
       <c r="Y20">
-        <v>0.3074310514321123</v>
+        <v>0.307469395749483</v>
       </c>
       <c r="Z20">
-        <v>0.2962797506424297</v>
+        <v>0.2962937016736581</v>
       </c>
       <c r="AA20">
-        <v>0.3105253606480539</v>
+        <v>0.3105184698495044</v>
       </c>
       <c r="AB20">
-        <v>0.2348122200185621</v>
+        <v>0.2348240657617434</v>
       </c>
     </row>
     <row r="21">
@@ -2206,82 +2206,82 @@
         </is>
       </c>
       <c r="B22">
-        <v>0.1864635482265845</v>
+        <v>0.1860749206471915</v>
       </c>
       <c r="C22">
-        <v>0.04305032799652037</v>
+        <v>0.04270461594735719</v>
       </c>
       <c r="D22">
-        <v>0.273645043390364</v>
+        <v>0.2736880457941302</v>
       </c>
       <c r="E22">
-        <v>0.2265620964953594</v>
+        <v>0.2266480702911372</v>
       </c>
       <c r="F22">
-        <v>0.01285106546278239</v>
+        <v>0.01263025020116457</v>
       </c>
       <c r="G22">
-        <v>0.005446595930337673</v>
+        <v>0.005582451479098068</v>
       </c>
       <c r="H22">
-        <v>0.05498920891964443</v>
+        <v>0.05571858693201029</v>
       </c>
       <c r="I22">
-        <v>0.2126854678990742</v>
+        <v>0.2124414934558372</v>
       </c>
       <c r="J22">
-        <v>0.1903735066941332</v>
+        <v>0.1900765496726321</v>
       </c>
       <c r="K22">
-        <v>0.114768702086555</v>
+        <v>0.1145027921456115</v>
       </c>
       <c r="L22">
-        <v>0.1172696897046826</v>
+        <v>0.1169420100048394</v>
       </c>
       <c r="M22">
-        <v>0.2309812695323909</v>
+        <v>0.2308717480747141</v>
       </c>
       <c r="N22">
-        <v>0.2314956670707393</v>
+        <v>0.2314141110879342</v>
       </c>
       <c r="O22">
-        <v>0.1143778684184701</v>
+        <v>0.1143822773826612</v>
       </c>
       <c r="P22">
-        <v>0.1974318804169292</v>
+        <v>0.1973406508596656</v>
       </c>
       <c r="Q22">
-        <v>0.10683661479572</v>
+        <v>0.1068761516923098</v>
       </c>
       <c r="R22">
-        <v>-0.07828055500257634</v>
+        <v>-0.07880303477807618</v>
       </c>
       <c r="S22">
-        <v>-0.09232738737452428</v>
+        <v>-0.0928560701431425</v>
       </c>
       <c r="T22">
-        <v>0.1261760819536201</v>
+        <v>0.1261521508710033</v>
       </c>
       <c r="U22">
         <v>0.0009227254258041933</v>
       </c>
       <c r="W22">
-        <v>0.3477836948570123</v>
+        <v>0.3476864501930671</v>
       </c>
       <c r="X22">
-        <v>0.2134318108081314</v>
+        <v>0.213228980230195</v>
       </c>
       <c r="Y22">
-        <v>0.206226417715522</v>
+        <v>0.2063582199614536</v>
       </c>
       <c r="Z22">
-        <v>0.2225998658736424</v>
+        <v>0.2226469068559747</v>
       </c>
       <c r="AA22">
-        <v>0.2105908404289103</v>
+        <v>0.2105321005094401</v>
       </c>
       <c r="AB22">
-        <v>0.2028482076155014</v>
+        <v>0.2028907417375988</v>
       </c>
     </row>
     <row r="23">
@@ -2291,82 +2291,82 @@
         </is>
       </c>
       <c r="B23">
-        <v>0.1854525588369179</v>
+        <v>0.1851961867736124</v>
       </c>
       <c r="C23">
-        <v>0.08298519338967646</v>
+        <v>0.08274346329636519</v>
       </c>
       <c r="D23">
-        <v>0.3849021664473969</v>
+        <v>0.3849391823768346</v>
       </c>
       <c r="E23">
-        <v>0.3304971738961116</v>
+        <v>0.3305675279571635</v>
       </c>
       <c r="F23">
-        <v>0.07291304573384587</v>
+        <v>0.0727622101567849</v>
       </c>
       <c r="G23">
-        <v>-0.1843850183102082</v>
+        <v>-0.184302951125371</v>
       </c>
       <c r="H23">
-        <v>0.03681155608437518</v>
+        <v>0.03734658138448063</v>
       </c>
       <c r="I23">
-        <v>0.2292670244879615</v>
+        <v>0.2291028197658982</v>
       </c>
       <c r="J23">
-        <v>0.2149581194945659</v>
+        <v>0.2147644491992538</v>
       </c>
       <c r="K23">
-        <v>0.01585083925799619</v>
+        <v>0.01563150988028812</v>
       </c>
       <c r="L23">
-        <v>-0.002920971674548827</v>
+        <v>-0.003203787163278293</v>
       </c>
       <c r="M23">
-        <v>0.2110854864861658</v>
+        <v>0.2110039610517267</v>
       </c>
       <c r="N23">
-        <v>0.208477323077658</v>
+        <v>0.2084157308403661</v>
       </c>
       <c r="O23">
-        <v>0.02419352604874877</v>
+        <v>0.02419368910670603</v>
       </c>
       <c r="P23">
-        <v>0.2070815185909677</v>
+        <v>0.2070137007676557</v>
       </c>
       <c r="Q23">
-        <v>0.1572623816922726</v>
+        <v>0.1572928563188545</v>
       </c>
       <c r="R23">
-        <v>0.1457812084915509</v>
+        <v>0.1455198349663011</v>
       </c>
       <c r="S23">
-        <v>0.1209896636107201</v>
+        <v>0.1207163207946081</v>
       </c>
       <c r="T23">
-        <v>0.1515094285417939</v>
+        <v>0.1514918092120514</v>
       </c>
       <c r="U23">
         <v>0.03547523441227284</v>
       </c>
       <c r="V23">
-        <v>0.3477836948570123</v>
+        <v>0.3476864501930671</v>
       </c>
       <c r="X23">
-        <v>0.2951695969295545</v>
+        <v>0.2950441056285603</v>
       </c>
       <c r="Y23">
-        <v>0.2100371499364326</v>
+        <v>0.2101373046847962</v>
       </c>
       <c r="Z23">
-        <v>0.3154662948021532</v>
+        <v>0.3155068272502439</v>
       </c>
       <c r="AA23">
-        <v>0.2827591001432633</v>
+        <v>0.2827217292141312</v>
       </c>
       <c r="AB23">
-        <v>0.2913126626982722</v>
+        <v>0.2913500539044127</v>
       </c>
     </row>
     <row r="24">
@@ -2376,82 +2376,82 @@
         </is>
       </c>
       <c r="B24">
-        <v>0.4140916042283412</v>
+        <v>0.4137782746922496</v>
       </c>
       <c r="C24">
-        <v>0.4506063187842265</v>
+        <v>0.4503507050477632</v>
       </c>
       <c r="D24">
-        <v>0.4534135614802932</v>
+        <v>0.4535036178197524</v>
       </c>
       <c r="E24">
-        <v>0.5120956148953959</v>
+        <v>0.5122562333475724</v>
       </c>
       <c r="F24">
-        <v>0.3828874406165315</v>
+        <v>0.3827171378420469</v>
       </c>
       <c r="G24">
-        <v>0.42934677532029</v>
+        <v>0.4295964277789796</v>
       </c>
       <c r="H24">
-        <v>0.1660969161404623</v>
+        <v>0.167118744581456</v>
       </c>
       <c r="I24">
-        <v>0.4206130835491929</v>
+        <v>0.4203893727952895</v>
       </c>
       <c r="J24">
-        <v>0.3722160446906417</v>
+        <v>0.3719322857189268</v>
       </c>
       <c r="K24">
-        <v>0.1358318361040546</v>
+        <v>0.1355090426346558</v>
       </c>
       <c r="L24">
-        <v>0.1063476770020601</v>
+        <v>0.105931356113506</v>
       </c>
       <c r="M24">
-        <v>0.2390575036400336</v>
+        <v>0.2389280818470994</v>
       </c>
       <c r="N24">
-        <v>0.2345165124716445</v>
+        <v>0.2344215023238028</v>
       </c>
       <c r="O24">
-        <v>0.06806584446781606</v>
+        <v>0.06806721577069377</v>
       </c>
       <c r="P24">
-        <v>0.4027671987637017</v>
+        <v>0.4026988190641543</v>
       </c>
       <c r="Q24">
-        <v>0.3028107849434409</v>
+        <v>0.3028899548277057</v>
       </c>
       <c r="R24">
-        <v>0.2550128996497166</v>
+        <v>0.2546362214002177</v>
       </c>
       <c r="S24">
-        <v>0.2814961750712565</v>
+        <v>0.2811295216726082</v>
       </c>
       <c r="T24">
-        <v>0.291850726205502</v>
+        <v>0.2918502019583458</v>
       </c>
       <c r="U24">
         <v>0.2811474278249858</v>
       </c>
       <c r="V24">
-        <v>0.2134318108081314</v>
+        <v>0.213228980230195</v>
       </c>
       <c r="W24">
-        <v>0.2951695969295545</v>
+        <v>0.2950441056285603</v>
       </c>
       <c r="Y24">
-        <v>0.6547927129891183</v>
+        <v>0.655038399630392</v>
       </c>
       <c r="Z24">
-        <v>0.8901688834086272</v>
+        <v>0.8903445549760043</v>
       </c>
       <c r="AA24">
-        <v>0.954023330534983</v>
+        <v>0.9540884319430374</v>
       </c>
       <c r="AB24">
-        <v>0.7113660230488882</v>
+        <v>0.711506700631415</v>
       </c>
     </row>
     <row r="25">
@@ -2461,82 +2461,82 @@
         </is>
       </c>
       <c r="B25">
-        <v>0.4115401023536915</v>
+        <v>0.4121078830032697</v>
       </c>
       <c r="C25">
-        <v>0.388035893846712</v>
+        <v>0.3882268416815529</v>
       </c>
       <c r="D25">
-        <v>0.3380539562958244</v>
+        <v>0.3380533127727982</v>
       </c>
       <c r="E25">
-        <v>0.3745800475602408</v>
+        <v>0.3745608377052729</v>
       </c>
       <c r="F25">
-        <v>0.3584276905542873</v>
+        <v>0.3585951886045599</v>
       </c>
       <c r="G25">
-        <v>0.7849799055840018</v>
+        <v>0.7849660069635523</v>
       </c>
       <c r="H25">
-        <v>0.1486366880162029</v>
+        <v>0.1484682200984068</v>
       </c>
       <c r="I25">
-        <v>0.3991283453381945</v>
+        <v>0.3993910979703796</v>
       </c>
       <c r="J25">
-        <v>0.3642934523720785</v>
+        <v>0.3646221304709235</v>
       </c>
       <c r="K25">
-        <v>0.2630782637138436</v>
+        <v>0.263296988813303</v>
       </c>
       <c r="L25">
-        <v>0.2423586880872797</v>
+        <v>0.2426416938901234</v>
       </c>
       <c r="M25">
-        <v>0.2097341033105758</v>
+        <v>0.2098212833323626</v>
       </c>
       <c r="N25">
-        <v>0.2063373161092445</v>
+        <v>0.2064034817014902</v>
       </c>
       <c r="O25">
-        <v>0.07022914083834858</v>
+        <v>0.07023256420821834</v>
       </c>
       <c r="P25">
-        <v>0.429196151826006</v>
+        <v>0.4293052952424644</v>
       </c>
       <c r="Q25">
-        <v>0.2913049507773651</v>
+        <v>0.2912993446265165</v>
       </c>
       <c r="R25">
-        <v>0.1761153044475365</v>
+        <v>0.1765187466263051</v>
       </c>
       <c r="S25">
-        <v>0.2228714859878356</v>
+        <v>0.2232979146494285</v>
       </c>
       <c r="T25">
-        <v>0.3074310514321123</v>
+        <v>0.307469395749483</v>
       </c>
       <c r="U25">
         <v>0.1149070673411441</v>
       </c>
       <c r="V25">
-        <v>0.206226417715522</v>
+        <v>0.2063582199614536</v>
       </c>
       <c r="W25">
-        <v>0.2100371499364326</v>
+        <v>0.2101373046847962</v>
       </c>
       <c r="X25">
-        <v>0.6547927129891183</v>
+        <v>0.655038399630392</v>
       </c>
       <c r="Z25">
-        <v>0.7238240501927573</v>
+        <v>0.7238269317650146</v>
       </c>
       <c r="AA25">
-        <v>0.6718590208962181</v>
+        <v>0.6719216750581058</v>
       </c>
       <c r="AB25">
-        <v>0.6826308504179501</v>
+        <v>0.6826332384779109</v>
       </c>
     </row>
     <row r="26">
@@ -2546,82 +2546,82 @@
         </is>
       </c>
       <c r="B26">
-        <v>0.4436045061227945</v>
+        <v>0.4439684890732144</v>
       </c>
       <c r="C26">
-        <v>0.4463002484186225</v>
+        <v>0.4463879454956496</v>
       </c>
       <c r="D26">
-        <v>0.4200868156564828</v>
+        <v>0.420085967507008</v>
       </c>
       <c r="E26">
-        <v>0.5008625715029008</v>
+        <v>0.5008610353124552</v>
       </c>
       <c r="F26">
-        <v>0.4338956528085992</v>
+        <v>0.4339741721117608</v>
       </c>
       <c r="G26">
-        <v>0.4859934247887432</v>
+        <v>0.4859926063769347</v>
       </c>
       <c r="H26">
-        <v>0.2109439578402317</v>
+        <v>0.2110968508457275</v>
       </c>
       <c r="I26">
-        <v>0.4547064339983174</v>
+        <v>0.4548509819244133</v>
       </c>
       <c r="J26">
-        <v>0.4033906328573477</v>
+        <v>0.4035747326591186</v>
       </c>
       <c r="K26">
-        <v>0.1426450415060509</v>
+        <v>0.142712643179018</v>
       </c>
       <c r="L26">
-        <v>0.09467593427367921</v>
+        <v>0.09475061337807365</v>
       </c>
       <c r="M26">
-        <v>0.2170902074544813</v>
+        <v>0.2171166148616001</v>
       </c>
       <c r="N26">
-        <v>0.2095966809277022</v>
+        <v>0.2096149304223076</v>
       </c>
       <c r="O26">
-        <v>0.03739113956807818</v>
+        <v>0.03739180388502106</v>
       </c>
       <c r="P26">
-        <v>0.3866910709182386</v>
+        <v>0.3867402416113038</v>
       </c>
       <c r="Q26">
-        <v>0.3211566183355837</v>
+        <v>0.321152607530685</v>
       </c>
       <c r="R26">
-        <v>0.301855794251151</v>
+        <v>0.3021549368649482</v>
       </c>
       <c r="S26">
-        <v>0.3350302487284268</v>
+        <v>0.3353452951229174</v>
       </c>
       <c r="T26">
-        <v>0.2962797506424297</v>
+        <v>0.2962937016736581</v>
       </c>
       <c r="U26">
         <v>0.2077622194335721</v>
       </c>
       <c r="V26">
-        <v>0.2225998658736424</v>
+        <v>0.2226469068559747</v>
       </c>
       <c r="W26">
-        <v>0.3154662948021532</v>
+        <v>0.3155068272502439</v>
       </c>
       <c r="X26">
-        <v>0.8901688834086272</v>
+        <v>0.8903445549760043</v>
       </c>
       <c r="Y26">
-        <v>0.7238240501927573</v>
+        <v>0.7238269317650146</v>
       </c>
       <c r="AA26">
-        <v>0.8752577411302238</v>
+        <v>0.8752832084666128</v>
       </c>
       <c r="AB26">
-        <v>0.7053109372562821</v>
+        <v>0.7053103115923237</v>
       </c>
     </row>
     <row r="27">
@@ -2631,82 +2631,82 @@
         </is>
       </c>
       <c r="B27">
-        <v>0.4395462282622183</v>
+        <v>0.4396399602828737</v>
       </c>
       <c r="C27">
-        <v>0.4922174989411097</v>
+        <v>0.4921496161070058</v>
       </c>
       <c r="D27">
-        <v>0.4661597273899097</v>
+        <v>0.466173422943744</v>
       </c>
       <c r="E27">
-        <v>0.5167626951529453</v>
+        <v>0.5168002527260575</v>
       </c>
       <c r="F27">
-        <v>0.402214976646558</v>
+        <v>0.4021799804074211</v>
       </c>
       <c r="G27">
-        <v>0.4527763585237524</v>
+        <v>0.4528490542911307</v>
       </c>
       <c r="H27">
-        <v>0.1606220018697473</v>
+        <v>0.1610634092400903</v>
       </c>
       <c r="I27">
-        <v>0.4403194251699888</v>
+        <v>0.4403050500102345</v>
       </c>
       <c r="J27">
-        <v>0.391116051336554</v>
+        <v>0.3911057785114367</v>
       </c>
       <c r="K27">
-        <v>0.1651244743268797</v>
+        <v>0.1650434677702124</v>
       </c>
       <c r="L27">
-        <v>0.1418886941619668</v>
+        <v>0.1417871818067766</v>
       </c>
       <c r="M27">
-        <v>0.2634668864320083</v>
+        <v>0.2634258936300762</v>
       </c>
       <c r="N27">
-        <v>0.2596212709662951</v>
+        <v>0.2595878516039381</v>
       </c>
       <c r="O27">
-        <v>0.08981717284198396</v>
+        <v>0.08981542741864301</v>
       </c>
       <c r="P27">
-        <v>0.4368691245825451</v>
+        <v>0.4368541251507124</v>
       </c>
       <c r="Q27">
-        <v>0.3171446190060881</v>
+        <v>0.3171560124960915</v>
       </c>
       <c r="R27">
-        <v>0.2707777589529218</v>
+        <v>0.2708006212946851</v>
       </c>
       <c r="S27">
-        <v>0.3013835204144575</v>
+        <v>0.301417717964827</v>
       </c>
       <c r="T27">
-        <v>0.3105253606480539</v>
+        <v>0.3105184698495044</v>
       </c>
       <c r="U27">
         <v>0.3104956334922062</v>
       </c>
       <c r="V27">
-        <v>0.2105908404289103</v>
+        <v>0.2105321005094401</v>
       </c>
       <c r="W27">
-        <v>0.2827591001432633</v>
+        <v>0.2827217292141312</v>
       </c>
       <c r="X27">
-        <v>0.954023330534983</v>
+        <v>0.9540884319430374</v>
       </c>
       <c r="Y27">
-        <v>0.6718590208962181</v>
+        <v>0.6719216750581058</v>
       </c>
       <c r="Z27">
-        <v>0.8752577411302238</v>
+        <v>0.8752832084666128</v>
       </c>
       <c r="AB27">
-        <v>0.7414290151700843</v>
+        <v>0.7414508965559262</v>
       </c>
     </row>
     <row r="28">
@@ -2716,82 +2716,82 @@
         </is>
       </c>
       <c r="B28">
-        <v>0.462922243465834</v>
+        <v>0.4632929735172144</v>
       </c>
       <c r="C28">
-        <v>0.4449190930416342</v>
+        <v>0.4449694344044621</v>
       </c>
       <c r="D28">
-        <v>0.4156772580361829</v>
+        <v>0.4156764728076081</v>
       </c>
       <c r="E28">
-        <v>0.4570231751505246</v>
+        <v>0.4570216054869827</v>
       </c>
       <c r="F28">
-        <v>0.3257244311566102</v>
+        <v>0.3257884068861948</v>
       </c>
       <c r="G28">
-        <v>0.4851280844945142</v>
+        <v>0.4851276754370418</v>
       </c>
       <c r="H28">
-        <v>0.09535162847028097</v>
+        <v>0.09538601469481374</v>
       </c>
       <c r="I28">
-        <v>0.4608884507285015</v>
+        <v>0.4610309462425894</v>
       </c>
       <c r="J28">
-        <v>0.4249354903462267</v>
+        <v>0.4251231670392321</v>
       </c>
       <c r="K28">
-        <v>0.2128236763995898</v>
+        <v>0.2129034349415712</v>
       </c>
       <c r="L28">
-        <v>0.1844911853384518</v>
+        <v>0.1845936274901514</v>
       </c>
       <c r="M28">
-        <v>0.2561259642933945</v>
+        <v>0.2561537760680311</v>
       </c>
       <c r="N28">
-        <v>0.2472411800837875</v>
+        <v>0.2472603294569372</v>
       </c>
       <c r="O28">
-        <v>0.06216503371454456</v>
+        <v>0.06216594163126758</v>
       </c>
       <c r="P28">
-        <v>0.3723253045936368</v>
+        <v>0.3723707059350114</v>
       </c>
       <c r="Q28">
-        <v>0.248237768223168</v>
+        <v>0.2482325913431211</v>
       </c>
       <c r="R28">
-        <v>0.253816369114977</v>
+        <v>0.2540893277464856</v>
       </c>
       <c r="S28">
-        <v>0.2812811894268327</v>
+        <v>0.2815588767505635</v>
       </c>
       <c r="T28">
-        <v>0.2348122200185621</v>
+        <v>0.2348240657617434</v>
       </c>
       <c r="U28">
         <v>0.2930197519048968</v>
       </c>
       <c r="V28">
-        <v>0.2028482076155014</v>
+        <v>0.2028907417375988</v>
       </c>
       <c r="W28">
-        <v>0.2913126626982722</v>
+        <v>0.2913500539044127</v>
       </c>
       <c r="X28">
-        <v>0.7113660230488882</v>
+        <v>0.711506700631415</v>
       </c>
       <c r="Y28">
-        <v>0.6826308504179501</v>
+        <v>0.6826332384779109</v>
       </c>
       <c r="Z28">
-        <v>0.7053109372562821</v>
+        <v>0.7053103115923237</v>
       </c>
       <c r="AA28">
-        <v>0.7414290151700843</v>
+        <v>0.7414508965559262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reflecting proper edits to headscan_full1 throughout all other documents, reknitting
</commit_message>
<xml_diff>
--- a/correlation_data_full.xlsx
+++ b/correlation_data_full.xlsx
@@ -518,10 +518,10 @@
         <v>0.3353035436244038</v>
       </c>
       <c r="G2">
-        <v>0.3236971878390013</v>
+        <v>0.3369063265926281</v>
       </c>
       <c r="H2">
-        <v>-0.0225201660993329</v>
+        <v>-0.02759663382889261</v>
       </c>
       <c r="I2">
         <v>0.8962132468714507</v>
@@ -542,13 +542,13 @@
         <v>0.4135145171964408</v>
       </c>
       <c r="O2">
-        <v>0.04719042423220197</v>
+        <v>0.05978041870211162</v>
       </c>
       <c r="P2">
         <v>0.2277054854577264</v>
       </c>
       <c r="Q2">
-        <v>0.04402615507213722</v>
+        <v>0.0395634327022626</v>
       </c>
       <c r="R2">
         <v>0.2213858907085259</v>
@@ -566,13 +566,13 @@
         <v>0.1860749206471915</v>
       </c>
       <c r="W2">
-        <v>0.1851961867736124</v>
+        <v>0.1877658152845463</v>
       </c>
       <c r="X2">
         <v>0.4137782746922496</v>
       </c>
       <c r="Y2">
-        <v>0.4121078830032697</v>
+        <v>0.4147640830302365</v>
       </c>
       <c r="Z2">
         <v>0.4439684890732144</v>
@@ -603,10 +603,10 @@
         <v>0.3032054674842555</v>
       </c>
       <c r="G3">
-        <v>0.3239964682391911</v>
+        <v>0.3642628980363894</v>
       </c>
       <c r="H3">
-        <v>0.05129771864827716</v>
+        <v>0.04435678048361254</v>
       </c>
       <c r="I3">
         <v>0.2550760362606682</v>
@@ -627,13 +627,13 @@
         <v>0.1213179227496275</v>
       </c>
       <c r="O3">
-        <v>0.07244794954821077</v>
+        <v>0.08229046563433723</v>
       </c>
       <c r="P3">
         <v>0.3011142612197973</v>
       </c>
       <c r="Q3">
-        <v>0.2373910808748982</v>
+        <v>0.2567708194717432</v>
       </c>
       <c r="R3">
         <v>0.1706431063113516</v>
@@ -651,13 +651,13 @@
         <v>0.04270461594735719</v>
       </c>
       <c r="W3">
-        <v>0.08274346329636519</v>
+        <v>0.07518881647752934</v>
       </c>
       <c r="X3">
         <v>0.4503507050477632</v>
       </c>
       <c r="Y3">
-        <v>0.3882268416815529</v>
+        <v>0.3987236269779414</v>
       </c>
       <c r="Z3">
         <v>0.4463879454956496</v>
@@ -688,10 +688,10 @@
         <v>0.1101013833874506</v>
       </c>
       <c r="G4">
-        <v>0.06573935776970632</v>
+        <v>0.08178532083093237</v>
       </c>
       <c r="H4">
-        <v>0.1916488558272403</v>
+        <v>0.1966794590637176</v>
       </c>
       <c r="I4">
         <v>0.2257782358420033</v>
@@ -712,13 +712,13 @@
         <v>0.2902305768007128</v>
       </c>
       <c r="O4">
-        <v>0.2835567453757912</v>
+        <v>0.2933527664426438</v>
       </c>
       <c r="P4">
         <v>0.5461144914187797</v>
       </c>
       <c r="Q4">
-        <v>0.5304458016652085</v>
+        <v>0.5441676452902511</v>
       </c>
       <c r="R4">
         <v>-0.1240677449488455</v>
@@ -736,13 +736,13 @@
         <v>0.2736880457941302</v>
       </c>
       <c r="W4">
-        <v>0.3849391823768346</v>
+        <v>0.3999202176911701</v>
       </c>
       <c r="X4">
         <v>0.4535036178197524</v>
       </c>
       <c r="Y4">
-        <v>0.3380533127727982</v>
+        <v>0.3311647159033571</v>
       </c>
       <c r="Z4">
         <v>0.420085967507008</v>
@@ -773,10 +773,10 @@
         <v>0.1442170072470644</v>
       </c>
       <c r="G5">
-        <v>0.1133672383287043</v>
+        <v>0.1385289126415964</v>
       </c>
       <c r="H5">
-        <v>0.2798484330095559</v>
+        <v>0.285477589184833</v>
       </c>
       <c r="I5">
         <v>0.1164079160348563</v>
@@ -797,13 +797,13 @@
         <v>0.124672080294903</v>
       </c>
       <c r="O5">
-        <v>0.2144749012938966</v>
+        <v>0.2224772257642394</v>
       </c>
       <c r="P5">
         <v>0.5086589493774576</v>
       </c>
       <c r="Q5">
-        <v>0.5794975316073759</v>
+        <v>0.6019254209528716</v>
       </c>
       <c r="R5">
         <v>-0.0918962480429867</v>
@@ -821,13 +821,13 @@
         <v>0.2266480702911372</v>
       </c>
       <c r="W5">
-        <v>0.3305675279571635</v>
+        <v>0.3457429837212002</v>
       </c>
       <c r="X5">
         <v>0.5122562333475724</v>
       </c>
       <c r="Y5">
-        <v>0.3745608377052729</v>
+        <v>0.375047223756918</v>
       </c>
       <c r="Z5">
         <v>0.5008610353124552</v>
@@ -858,10 +858,10 @@
         <v>0.1442170072470644</v>
       </c>
       <c r="G6">
-        <v>0.3177272721685255</v>
+        <v>0.3502331002612809</v>
       </c>
       <c r="H6">
-        <v>-0.03510670429895189</v>
+        <v>-0.0346491989303611</v>
       </c>
       <c r="I6">
         <v>0.3308874443691532</v>
@@ -882,13 +882,13 @@
         <v>0.08909260643959102</v>
       </c>
       <c r="O6">
-        <v>0.0531505027449837</v>
+        <v>0.06530966786775173</v>
       </c>
       <c r="P6">
         <v>0.2122622921001213</v>
       </c>
       <c r="Q6">
-        <v>0.1736201616372676</v>
+        <v>0.1756102404887688</v>
       </c>
       <c r="R6">
         <v>0.3054321938811898</v>
@@ -906,13 +906,13 @@
         <v>0.01263025020116457</v>
       </c>
       <c r="W6">
-        <v>0.0727622101567849</v>
+        <v>0.07452776713627086</v>
       </c>
       <c r="X6">
         <v>0.3827171378420469</v>
       </c>
       <c r="Y6">
-        <v>0.3585951886045599</v>
+        <v>0.3660074469456079</v>
       </c>
       <c r="Z6">
         <v>0.4339741721117608</v>
@@ -931,82 +931,82 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.3236971878390013</v>
+        <v>0.3369063265926281</v>
       </c>
       <c r="C7">
-        <v>0.3239964682391911</v>
+        <v>0.3642628980363894</v>
       </c>
       <c r="D7">
-        <v>0.06573935776970632</v>
+        <v>0.08178532083093237</v>
       </c>
       <c r="E7">
-        <v>0.1133672383287043</v>
+        <v>0.1385289126415964</v>
       </c>
       <c r="F7">
-        <v>0.3177272721685255</v>
+        <v>0.3502331002612809</v>
       </c>
       <c r="H7">
-        <v>0.02149030032071721</v>
+        <v>0.02842854742900396</v>
       </c>
       <c r="I7">
-        <v>0.2828530216981644</v>
+        <v>0.2990948378136545</v>
       </c>
       <c r="J7">
-        <v>0.2640401896402293</v>
+        <v>0.2807759031282003</v>
       </c>
       <c r="K7">
-        <v>0.2614278969556863</v>
+        <v>0.2840139339639582</v>
       </c>
       <c r="L7">
-        <v>0.2604577249577279</v>
+        <v>0.277701799782818</v>
       </c>
       <c r="M7">
-        <v>0.08513926640104709</v>
+        <v>0.07440409671582113</v>
       </c>
       <c r="N7">
-        <v>0.08045849328625392</v>
+        <v>0.07013454886547639</v>
       </c>
       <c r="O7">
-        <v>0.01816571709808065</v>
+        <v>0.01228480365016764</v>
       </c>
       <c r="P7">
-        <v>0.218694363545172</v>
+        <v>0.2446013583671175</v>
       </c>
       <c r="Q7">
-        <v>0.1062571623805989</v>
+        <v>0.1366099553063804</v>
       </c>
       <c r="R7">
-        <v>0.1711986253962139</v>
+        <v>0.1528326555956195</v>
       </c>
       <c r="S7">
-        <v>0.2105637122323289</v>
+        <v>0.1979993058006543</v>
       </c>
       <c r="T7">
-        <v>0.1201756373706857</v>
+        <v>0.1461533141461698</v>
       </c>
       <c r="U7">
-        <v>0.1762047123370334</v>
+        <v>0.1801322213206275</v>
       </c>
       <c r="V7">
-        <v>0.005582451479098068</v>
+        <v>0.01325754104619871</v>
       </c>
       <c r="W7">
-        <v>-0.184302951125371</v>
+        <v>-0.2363991004814481</v>
       </c>
       <c r="X7">
-        <v>0.4295964277789796</v>
+        <v>0.469773696608588</v>
       </c>
       <c r="Y7">
-        <v>0.7849660069635523</v>
+        <v>0.8045217090672854</v>
       </c>
       <c r="Z7">
-        <v>0.4859926063769347</v>
+        <v>0.5454359547554969</v>
       </c>
       <c r="AA7">
-        <v>0.4528490542911307</v>
+        <v>0.4998591441028649</v>
       </c>
       <c r="AB7">
-        <v>0.4851276754370418</v>
+        <v>0.5296781271196432</v>
       </c>
     </row>
     <row r="8">
@@ -1016,82 +1016,82 @@
         </is>
       </c>
       <c r="B8">
-        <v>-0.0225201660993329</v>
+        <v>-0.02759663382889261</v>
       </c>
       <c r="C8">
-        <v>0.05129771864827716</v>
+        <v>0.04435678048361254</v>
       </c>
       <c r="D8">
-        <v>0.1916488558272403</v>
+        <v>0.1966794590637176</v>
       </c>
       <c r="E8">
-        <v>0.2798484330095559</v>
+        <v>0.285477589184833</v>
       </c>
       <c r="F8">
-        <v>-0.03510670429895189</v>
+        <v>-0.0346491989303611</v>
       </c>
       <c r="G8">
-        <v>0.02149030032071721</v>
+        <v>0.02842854742900396</v>
       </c>
       <c r="I8">
-        <v>-0.01892143169657567</v>
+        <v>-0.02341978667370561</v>
       </c>
       <c r="J8">
-        <v>-0.075132651862499</v>
+        <v>-0.08063386203089389</v>
       </c>
       <c r="K8">
-        <v>-0.1197490619453794</v>
+        <v>-0.1234323232961675</v>
       </c>
       <c r="L8">
-        <v>-0.113950251193763</v>
+        <v>-0.1194013037897156</v>
       </c>
       <c r="M8">
-        <v>-0.07818098883018644</v>
+        <v>-0.07434571563573382</v>
       </c>
       <c r="N8">
-        <v>-0.07628804370444969</v>
+        <v>-0.07287921669042526</v>
       </c>
       <c r="O8">
-        <v>0.01424452783182506</v>
+        <v>0.01386612412697811</v>
       </c>
       <c r="P8">
-        <v>0.275885638251716</v>
+        <v>0.2774148975252184</v>
       </c>
       <c r="Q8">
-        <v>0.3502217670037115</v>
+        <v>0.3628242646819061</v>
       </c>
       <c r="R8">
-        <v>-0.1656944313144815</v>
+        <v>-0.1686050786559357</v>
       </c>
       <c r="S8">
-        <v>-0.1279764998732663</v>
+        <v>-0.1292575478199528</v>
       </c>
       <c r="T8">
-        <v>0.348997943631939</v>
+        <v>0.3516079377193551</v>
       </c>
       <c r="U8">
-        <v>-0.2131799171230018</v>
+        <v>-0.2262761290344947</v>
       </c>
       <c r="V8">
-        <v>0.05571858693201029</v>
+        <v>0.05754428796409604</v>
       </c>
       <c r="W8">
-        <v>0.03734658138448063</v>
+        <v>0.04673302774292012</v>
       </c>
       <c r="X8">
-        <v>0.167118744581456</v>
+        <v>0.1648612055399581</v>
       </c>
       <c r="Y8">
-        <v>0.1484682200984068</v>
+        <v>0.1501384835258873</v>
       </c>
       <c r="Z8">
-        <v>0.2110968508457275</v>
+        <v>0.2107718546467774</v>
       </c>
       <c r="AA8">
-        <v>0.1610634092400903</v>
+        <v>0.1574077995753776</v>
       </c>
       <c r="AB8">
-        <v>0.09538601469481374</v>
+        <v>0.08336182079441845</v>
       </c>
     </row>
     <row r="9">
@@ -1116,10 +1116,10 @@
         <v>0.3308874443691532</v>
       </c>
       <c r="G9">
-        <v>0.2828530216981644</v>
+        <v>0.2990948378136545</v>
       </c>
       <c r="H9">
-        <v>-0.01892143169657567</v>
+        <v>-0.02341978667370561</v>
       </c>
       <c r="J9">
         <v>0.9712376187738408</v>
@@ -1137,13 +1137,13 @@
         <v>0.4221636708752149</v>
       </c>
       <c r="O9">
-        <v>0.07874567696688811</v>
+        <v>0.09330207095356544</v>
       </c>
       <c r="P9">
         <v>0.2568221946204033</v>
       </c>
       <c r="Q9">
-        <v>0.09753912176323662</v>
+        <v>0.09287306121429487</v>
       </c>
       <c r="R9">
         <v>0.1908115306086125</v>
@@ -1161,13 +1161,13 @@
         <v>0.2124414934558372</v>
       </c>
       <c r="W9">
-        <v>0.2291028197658982</v>
+        <v>0.2332344048041308</v>
       </c>
       <c r="X9">
         <v>0.4203893727952895</v>
       </c>
       <c r="Y9">
-        <v>0.3993910979703796</v>
+        <v>0.3995156128751827</v>
       </c>
       <c r="Z9">
         <v>0.4548509819244133</v>
@@ -1201,10 +1201,10 @@
         <v>0.3083242242546798</v>
       </c>
       <c r="G10">
-        <v>0.2640401896402293</v>
+        <v>0.2807759031282003</v>
       </c>
       <c r="H10">
-        <v>-0.075132651862499</v>
+        <v>-0.08063386203089389</v>
       </c>
       <c r="I10">
         <v>0.9712376187738408</v>
@@ -1222,13 +1222,13 @@
         <v>0.4077082805258652</v>
       </c>
       <c r="O10">
-        <v>0.05671414325509426</v>
+        <v>0.0709232024722083</v>
       </c>
       <c r="P10">
         <v>0.2007180287572574</v>
       </c>
       <c r="Q10">
-        <v>0.02918843718686302</v>
+        <v>0.02295938913463506</v>
       </c>
       <c r="R10">
         <v>0.2119291190826943</v>
@@ -1246,13 +1246,13 @@
         <v>0.1900765496726321</v>
       </c>
       <c r="W10">
-        <v>0.2147644491992538</v>
+        <v>0.2174749294945283</v>
       </c>
       <c r="X10">
         <v>0.3719322857189268</v>
       </c>
       <c r="Y10">
-        <v>0.3646221304709235</v>
+        <v>0.3639976909010245</v>
       </c>
       <c r="Z10">
         <v>0.4035747326591186</v>
@@ -1286,10 +1286,10 @@
         <v>0.1755517833373934</v>
       </c>
       <c r="G11">
-        <v>0.2614278969556863</v>
+        <v>0.2840139339639582</v>
       </c>
       <c r="H11">
-        <v>-0.1197490619453794</v>
+        <v>-0.1234323232961675</v>
       </c>
       <c r="I11">
         <v>0.4378938308009257</v>
@@ -1307,13 +1307,13 @@
         <v>0.1927308280386089</v>
       </c>
       <c r="O11">
-        <v>0.05124348000204136</v>
+        <v>0.0637292450642422</v>
       </c>
       <c r="P11">
         <v>0.09969716055863168</v>
       </c>
       <c r="Q11">
-        <v>-0.04540124905632316</v>
+        <v>-0.04759887357887706</v>
       </c>
       <c r="R11">
         <v>0.1484653638711309</v>
@@ -1331,13 +1331,13 @@
         <v>0.1145027921456115</v>
       </c>
       <c r="W11">
-        <v>0.01563150988028812</v>
+        <v>0.01439023441647101</v>
       </c>
       <c r="X11">
         <v>0.1355090426346558</v>
       </c>
       <c r="Y11">
-        <v>0.263296988813303</v>
+        <v>0.2624880755695151</v>
       </c>
       <c r="Z11">
         <v>0.142712643179018</v>
@@ -1371,10 +1371,10 @@
         <v>0.1337497712722012</v>
       </c>
       <c r="G12">
-        <v>0.2604577249577279</v>
+        <v>0.277701799782818</v>
       </c>
       <c r="H12">
-        <v>-0.113950251193763</v>
+        <v>-0.1194013037897156</v>
       </c>
       <c r="I12">
         <v>0.419327418664915</v>
@@ -1392,13 +1392,13 @@
         <v>0.1872742694289936</v>
       </c>
       <c r="O12">
-        <v>0.04923288234022009</v>
+        <v>0.06187490279114954</v>
       </c>
       <c r="P12">
         <v>0.1041883253381078</v>
       </c>
       <c r="Q12">
-        <v>-0.07516055710950412</v>
+        <v>-0.07981620181669503</v>
       </c>
       <c r="R12">
         <v>0.1191647463280724</v>
@@ -1416,13 +1416,13 @@
         <v>0.1169420100048394</v>
       </c>
       <c r="W12">
-        <v>-0.003203787163278293</v>
+        <v>-0.005663670117834274</v>
       </c>
       <c r="X12">
         <v>0.105931356113506</v>
       </c>
       <c r="Y12">
-        <v>0.2426416938901234</v>
+        <v>0.2396702670209695</v>
       </c>
       <c r="Z12">
         <v>0.09475061337807365</v>
@@ -1456,10 +1456,10 @@
         <v>0.09301441959147191</v>
       </c>
       <c r="G13">
-        <v>0.08513926640104709</v>
+        <v>0.07440409671582113</v>
       </c>
       <c r="H13">
-        <v>-0.07818098883018644</v>
+        <v>-0.07434571563573382</v>
       </c>
       <c r="I13">
         <v>0.4311387230466044</v>
@@ -1477,13 +1477,13 @@
         <v>0.9930601937599935</v>
       </c>
       <c r="O13">
-        <v>0.4814443693986965</v>
+        <v>0.556110920418823</v>
       </c>
       <c r="P13">
         <v>0.4982138529267472</v>
       </c>
       <c r="Q13">
-        <v>0.1192758446805697</v>
+        <v>0.1171519526717874</v>
       </c>
       <c r="R13">
         <v>-0.03441708348787718</v>
@@ -1501,13 +1501,13 @@
         <v>0.2308717480747141</v>
       </c>
       <c r="W13">
-        <v>0.2110039610517267</v>
+        <v>0.2231103204226994</v>
       </c>
       <c r="X13">
         <v>0.2389280818470994</v>
       </c>
       <c r="Y13">
-        <v>0.2098212833323626</v>
+        <v>0.209351249320094</v>
       </c>
       <c r="Z13">
         <v>0.2171166148616001</v>
@@ -1541,10 +1541,10 @@
         <v>0.08909260643959102</v>
       </c>
       <c r="G14">
-        <v>0.08045849328625392</v>
+        <v>0.07013454886547639</v>
       </c>
       <c r="H14">
-        <v>-0.07628804370444969</v>
+        <v>-0.07287921669042526</v>
       </c>
       <c r="I14">
         <v>0.4221636708752149</v>
@@ -1562,13 +1562,13 @@
         <v>0.9930601937599935</v>
       </c>
       <c r="O14">
-        <v>0.4867230732292473</v>
+        <v>0.5649804693663774</v>
       </c>
       <c r="P14">
         <v>0.5073508488973718</v>
       </c>
       <c r="Q14">
-        <v>0.1189792709547957</v>
+        <v>0.117315129888777</v>
       </c>
       <c r="R14">
         <v>-0.04172526642003677</v>
@@ -1586,13 +1586,13 @@
         <v>0.2314141110879342</v>
       </c>
       <c r="W14">
-        <v>0.2084157308403661</v>
+        <v>0.2213009469773712</v>
       </c>
       <c r="X14">
         <v>0.2344215023238028</v>
       </c>
       <c r="Y14">
-        <v>0.2064034817014902</v>
+        <v>0.20516076838721</v>
       </c>
       <c r="Z14">
         <v>0.2096149304223076</v>
@@ -1611,82 +1611,82 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.04719042423220197</v>
+        <v>0.05978041870211162</v>
       </c>
       <c r="C15">
-        <v>0.07244794954821077</v>
+        <v>0.08229046563433723</v>
       </c>
       <c r="D15">
-        <v>0.2835567453757912</v>
+        <v>0.2933527664426438</v>
       </c>
       <c r="E15">
-        <v>0.2144749012938966</v>
+        <v>0.2224772257642394</v>
       </c>
       <c r="F15">
-        <v>0.0531505027449837</v>
+        <v>0.06530966786775173</v>
       </c>
       <c r="G15">
-        <v>0.01816571709808065</v>
+        <v>0.01228480365016764</v>
       </c>
       <c r="H15">
-        <v>0.01424452783182506</v>
+        <v>0.01386612412697811</v>
       </c>
       <c r="I15">
-        <v>0.07874567696688811</v>
+        <v>0.09330207095356544</v>
       </c>
       <c r="J15">
-        <v>0.05671414325509426</v>
+        <v>0.0709232024722083</v>
       </c>
       <c r="K15">
-        <v>0.05124348000204136</v>
+        <v>0.0637292450642422</v>
       </c>
       <c r="L15">
-        <v>0.04923288234022009</v>
+        <v>0.06187490279114954</v>
       </c>
       <c r="M15">
-        <v>0.4814443693986965</v>
+        <v>0.556110920418823</v>
       </c>
       <c r="N15">
-        <v>0.4867230732292473</v>
+        <v>0.5649804693663774</v>
       </c>
       <c r="P15">
-        <v>0.3751519894817744</v>
+        <v>0.4378019468062452</v>
       </c>
       <c r="Q15">
-        <v>0.2270249835937784</v>
+        <v>0.2415135358589916</v>
       </c>
       <c r="R15">
-        <v>-0.1576871134965886</v>
+        <v>-0.1525669431901946</v>
       </c>
       <c r="S15">
-        <v>-0.1149810790924108</v>
+        <v>-0.105669554314247</v>
       </c>
       <c r="T15">
-        <v>0.2557265663160282</v>
+        <v>0.2679599545219127</v>
       </c>
       <c r="U15">
-        <v>-0.1173516718667757</v>
+        <v>-0.1003708712144724</v>
       </c>
       <c r="V15">
-        <v>0.1143822773826612</v>
+        <v>0.1132684023566317</v>
       </c>
       <c r="W15">
-        <v>0.02419368910670603</v>
+        <v>0.04882179840989144</v>
       </c>
       <c r="X15">
-        <v>0.06806721577069377</v>
+        <v>0.08376128976985853</v>
       </c>
       <c r="Y15">
-        <v>0.07023256420821834</v>
+        <v>0.08081703698659988</v>
       </c>
       <c r="Z15">
-        <v>0.03739180388502106</v>
+        <v>0.05511792127583255</v>
       </c>
       <c r="AA15">
-        <v>0.08981542741864301</v>
+        <v>0.1097013220610039</v>
       </c>
       <c r="AB15">
-        <v>0.06216594163126758</v>
+        <v>0.07060253827758957</v>
       </c>
     </row>
     <row r="16">
@@ -1711,10 +1711,10 @@
         <v>0.2122622921001213</v>
       </c>
       <c r="G16">
-        <v>0.218694363545172</v>
+        <v>0.2446013583671175</v>
       </c>
       <c r="H16">
-        <v>0.275885638251716</v>
+        <v>0.2774148975252184</v>
       </c>
       <c r="I16">
         <v>0.2568221946204033</v>
@@ -1735,10 +1735,10 @@
         <v>0.5073508488973718</v>
       </c>
       <c r="O16">
-        <v>0.3751519894817744</v>
+        <v>0.4378019468062452</v>
       </c>
       <c r="Q16">
-        <v>0.8020419371435977</v>
+        <v>0.8081860151953411</v>
       </c>
       <c r="R16">
         <v>-0.1014788246072017</v>
@@ -1756,13 +1756,13 @@
         <v>0.1973406508596656</v>
       </c>
       <c r="W16">
-        <v>0.2070137007676557</v>
+        <v>0.222101154067763</v>
       </c>
       <c r="X16">
         <v>0.4026988190641543</v>
       </c>
       <c r="Y16">
-        <v>0.4293052952424644</v>
+        <v>0.4345783050997502</v>
       </c>
       <c r="Z16">
         <v>0.3867402416113038</v>
@@ -1781,82 +1781,82 @@
         </is>
       </c>
       <c r="B17">
-        <v>0.04402615507213722</v>
+        <v>0.0395634327022626</v>
       </c>
       <c r="C17">
-        <v>0.2373910808748982</v>
+        <v>0.2567708194717432</v>
       </c>
       <c r="D17">
-        <v>0.5304458016652085</v>
+        <v>0.5441676452902511</v>
       </c>
       <c r="E17">
-        <v>0.5794975316073759</v>
+        <v>0.6019254209528716</v>
       </c>
       <c r="F17">
-        <v>0.1736201616372676</v>
+        <v>0.1756102404887688</v>
       </c>
       <c r="G17">
-        <v>0.1062571623805989</v>
+        <v>0.1366099553063804</v>
       </c>
       <c r="H17">
-        <v>0.3502217670037115</v>
+        <v>0.3628242646819061</v>
       </c>
       <c r="I17">
-        <v>0.09753912176323662</v>
+        <v>0.09287306121429487</v>
       </c>
       <c r="J17">
-        <v>0.02918843718686302</v>
+        <v>0.02295938913463506</v>
       </c>
       <c r="K17">
-        <v>-0.04540124905632316</v>
+        <v>-0.04759887357887706</v>
       </c>
       <c r="L17">
-        <v>-0.07516055710950412</v>
+        <v>-0.07981620181669503</v>
       </c>
       <c r="M17">
-        <v>0.1192758446805697</v>
+        <v>0.1171519526717874</v>
       </c>
       <c r="N17">
-        <v>0.1189792709547957</v>
+        <v>0.117315129888777</v>
       </c>
       <c r="O17">
-        <v>0.2270249835937784</v>
+        <v>0.2415135358589916</v>
       </c>
       <c r="P17">
-        <v>0.8020419371435977</v>
+        <v>0.8081860151953411</v>
       </c>
       <c r="R17">
-        <v>-0.143430232537778</v>
+        <v>-0.1730404339624289</v>
       </c>
       <c r="S17">
-        <v>-0.0778411579523758</v>
+        <v>-0.1060010172985709</v>
       </c>
       <c r="T17">
-        <v>0.9466253699514651</v>
+        <v>0.9452761297779024</v>
       </c>
       <c r="U17">
-        <v>-0.1799687160309316</v>
+        <v>-0.1807436460765975</v>
       </c>
       <c r="V17">
-        <v>0.1068761516923098</v>
+        <v>0.1128299314290781</v>
       </c>
       <c r="W17">
-        <v>0.1572928563188545</v>
+        <v>0.1712911512420745</v>
       </c>
       <c r="X17">
-        <v>0.3028899548277057</v>
+        <v>0.3082769415170779</v>
       </c>
       <c r="Y17">
-        <v>0.2912993446265165</v>
+        <v>0.3022942318695974</v>
       </c>
       <c r="Z17">
-        <v>0.321152607530685</v>
+        <v>0.3287255710913217</v>
       </c>
       <c r="AA17">
-        <v>0.3171560124960915</v>
+        <v>0.3254635300179367</v>
       </c>
       <c r="AB17">
-        <v>0.2482325913431211</v>
+        <v>0.2535248071666839</v>
       </c>
     </row>
     <row r="18">
@@ -1881,10 +1881,10 @@
         <v>0.3054321938811898</v>
       </c>
       <c r="G18">
-        <v>0.1711986253962139</v>
+        <v>0.1528326555956195</v>
       </c>
       <c r="H18">
-        <v>-0.1656944313144815</v>
+        <v>-0.1686050786559357</v>
       </c>
       <c r="I18">
         <v>0.1908115306086125</v>
@@ -1905,13 +1905,13 @@
         <v>-0.04172526642003677</v>
       </c>
       <c r="O18">
-        <v>-0.1576871134965886</v>
+        <v>-0.1525669431901946</v>
       </c>
       <c r="P18">
         <v>-0.1014788246072017</v>
       </c>
       <c r="Q18">
-        <v>-0.143430232537778</v>
+        <v>-0.1730404339624289</v>
       </c>
       <c r="S18">
         <v>0.9613207253471929</v>
@@ -1926,13 +1926,13 @@
         <v>-0.07880303477807618</v>
       </c>
       <c r="W18">
-        <v>0.1455198349663011</v>
+        <v>0.09390252887980635</v>
       </c>
       <c r="X18">
         <v>0.2546362214002177</v>
       </c>
       <c r="Y18">
-        <v>0.1765187466263051</v>
+        <v>0.181958816909036</v>
       </c>
       <c r="Z18">
         <v>0.3021549368649482</v>
@@ -1966,10 +1966,10 @@
         <v>0.326391697294726</v>
       </c>
       <c r="G19">
-        <v>0.2105637122323289</v>
+        <v>0.1979993058006543</v>
       </c>
       <c r="H19">
-        <v>-0.1279764998732663</v>
+        <v>-0.1292575478199528</v>
       </c>
       <c r="I19">
         <v>0.1740021193325153</v>
@@ -1990,13 +1990,13 @@
         <v>-0.04017403757573355</v>
       </c>
       <c r="O19">
-        <v>-0.1149810790924108</v>
+        <v>-0.105669554314247</v>
       </c>
       <c r="P19">
         <v>-0.03615342245176581</v>
       </c>
       <c r="Q19">
-        <v>-0.0778411579523758</v>
+        <v>-0.1060010172985709</v>
       </c>
       <c r="R19">
         <v>0.9613207253471929</v>
@@ -2011,13 +2011,13 @@
         <v>-0.0928560701431425</v>
       </c>
       <c r="W19">
-        <v>0.1207163207946081</v>
+        <v>0.06754019836006939</v>
       </c>
       <c r="X19">
         <v>0.2811295216726082</v>
       </c>
       <c r="Y19">
-        <v>0.2232979146494285</v>
+        <v>0.2294283773148871</v>
       </c>
       <c r="Z19">
         <v>0.3353452951229174</v>
@@ -2051,10 +2051,10 @@
         <v>0.1441245155244848</v>
       </c>
       <c r="G20">
-        <v>0.1201756373706857</v>
+        <v>0.1461533141461698</v>
       </c>
       <c r="H20">
-        <v>0.348997943631939</v>
+        <v>0.3516079377193551</v>
       </c>
       <c r="I20">
         <v>0.07218036953787371</v>
@@ -2075,13 +2075,13 @@
         <v>0.153680112528515</v>
       </c>
       <c r="O20">
-        <v>0.2557265663160282</v>
+        <v>0.2679599545219127</v>
       </c>
       <c r="P20">
         <v>0.8641310656617663</v>
       </c>
       <c r="Q20">
-        <v>0.9466253699514651</v>
+        <v>0.9452761297779024</v>
       </c>
       <c r="R20">
         <v>-0.1694610076243347</v>
@@ -2096,13 +2096,13 @@
         <v>0.1261521508710033</v>
       </c>
       <c r="W20">
-        <v>0.1514918092120514</v>
+        <v>0.1653826925730575</v>
       </c>
       <c r="X20">
         <v>0.2918502019583458</v>
       </c>
       <c r="Y20">
-        <v>0.307469395749483</v>
+        <v>0.313423316448216</v>
       </c>
       <c r="Z20">
         <v>0.2962937016736581</v>
@@ -2136,10 +2136,10 @@
         <v>0.1574296744346301</v>
       </c>
       <c r="G21">
-        <v>0.1762047123370334</v>
+        <v>0.1801322213206275</v>
       </c>
       <c r="H21">
-        <v>-0.2131799171230018</v>
+        <v>-0.2262761290344947</v>
       </c>
       <c r="I21">
         <v>0.2773549624024398</v>
@@ -2160,13 +2160,13 @@
         <v>0.08802685745852554</v>
       </c>
       <c r="O21">
-        <v>-0.1173516718667757</v>
+        <v>-0.1003708712144724</v>
       </c>
       <c r="P21">
         <v>-0.08868916681725575</v>
       </c>
       <c r="Q21">
-        <v>-0.1799687160309316</v>
+        <v>-0.1807436460765975</v>
       </c>
       <c r="R21">
         <v>0.3184190306397158</v>
@@ -2181,13 +2181,13 @@
         <v>0.0009227254258041933</v>
       </c>
       <c r="W21">
-        <v>0.03547523441227284</v>
+        <v>0.01675869359039526</v>
       </c>
       <c r="X21">
         <v>0.2811474278249858</v>
       </c>
       <c r="Y21">
-        <v>0.1149070673411441</v>
+        <v>0.1145405512611248</v>
       </c>
       <c r="Z21">
         <v>0.2077622194335721</v>
@@ -2221,10 +2221,10 @@
         <v>0.01263025020116457</v>
       </c>
       <c r="G22">
-        <v>0.005582451479098068</v>
+        <v>0.01325754104619871</v>
       </c>
       <c r="H22">
-        <v>0.05571858693201029</v>
+        <v>0.05754428796409604</v>
       </c>
       <c r="I22">
         <v>0.2124414934558372</v>
@@ -2245,13 +2245,13 @@
         <v>0.2314141110879342</v>
       </c>
       <c r="O22">
-        <v>0.1143822773826612</v>
+        <v>0.1132684023566317</v>
       </c>
       <c r="P22">
         <v>0.1973406508596656</v>
       </c>
       <c r="Q22">
-        <v>0.1068761516923098</v>
+        <v>0.1128299314290781</v>
       </c>
       <c r="R22">
         <v>-0.07880303477807618</v>
@@ -2266,13 +2266,13 @@
         <v>0.0009227254258041933</v>
       </c>
       <c r="W22">
-        <v>0.3476864501930671</v>
+        <v>0.3635434921086566</v>
       </c>
       <c r="X22">
         <v>0.213228980230195</v>
       </c>
       <c r="Y22">
-        <v>0.2063582199614536</v>
+        <v>0.2049644406841535</v>
       </c>
       <c r="Z22">
         <v>0.2226469068559747</v>
@@ -2291,82 +2291,82 @@
         </is>
       </c>
       <c r="B23">
-        <v>0.1851961867736124</v>
+        <v>0.1877658152845463</v>
       </c>
       <c r="C23">
-        <v>0.08274346329636519</v>
+        <v>0.07518881647752934</v>
       </c>
       <c r="D23">
-        <v>0.3849391823768346</v>
+        <v>0.3999202176911701</v>
       </c>
       <c r="E23">
-        <v>0.3305675279571635</v>
+        <v>0.3457429837212002</v>
       </c>
       <c r="F23">
-        <v>0.0727622101567849</v>
+        <v>0.07452776713627086</v>
       </c>
       <c r="G23">
-        <v>-0.184302951125371</v>
+        <v>-0.2363991004814481</v>
       </c>
       <c r="H23">
-        <v>0.03734658138448063</v>
+        <v>0.04673302774292012</v>
       </c>
       <c r="I23">
-        <v>0.2291028197658982</v>
+        <v>0.2332344048041308</v>
       </c>
       <c r="J23">
-        <v>0.2147644491992538</v>
+        <v>0.2174749294945283</v>
       </c>
       <c r="K23">
-        <v>0.01563150988028812</v>
+        <v>0.01439023441647101</v>
       </c>
       <c r="L23">
-        <v>-0.003203787163278293</v>
+        <v>-0.005663670117834274</v>
       </c>
       <c r="M23">
-        <v>0.2110039610517267</v>
+        <v>0.2231103204226994</v>
       </c>
       <c r="N23">
-        <v>0.2084157308403661</v>
+        <v>0.2213009469773712</v>
       </c>
       <c r="O23">
-        <v>0.02419368910670603</v>
+        <v>0.04882179840989144</v>
       </c>
       <c r="P23">
-        <v>0.2070137007676557</v>
+        <v>0.222101154067763</v>
       </c>
       <c r="Q23">
-        <v>0.1572928563188545</v>
+        <v>0.1712911512420745</v>
       </c>
       <c r="R23">
-        <v>0.1455198349663011</v>
+        <v>0.09390252887980635</v>
       </c>
       <c r="S23">
-        <v>0.1207163207946081</v>
+        <v>0.06754019836006939</v>
       </c>
       <c r="T23">
-        <v>0.1514918092120514</v>
+        <v>0.1653826925730575</v>
       </c>
       <c r="U23">
-        <v>0.03547523441227284</v>
+        <v>0.01675869359039526</v>
       </c>
       <c r="V23">
-        <v>0.3476864501930671</v>
+        <v>0.3635434921086566</v>
       </c>
       <c r="X23">
-        <v>0.2950441056285603</v>
+        <v>0.3116652659886188</v>
       </c>
       <c r="Y23">
-        <v>0.2101373046847962</v>
+        <v>0.2732065978799744</v>
       </c>
       <c r="Z23">
-        <v>0.3155068272502439</v>
+        <v>0.3279898868767614</v>
       </c>
       <c r="AA23">
-        <v>0.2827217292141312</v>
+        <v>0.2971741056403512</v>
       </c>
       <c r="AB23">
-        <v>0.2913500539044127</v>
+        <v>0.3006944690630143</v>
       </c>
     </row>
     <row r="24">
@@ -2391,10 +2391,10 @@
         <v>0.3827171378420469</v>
       </c>
       <c r="G24">
-        <v>0.4295964277789796</v>
+        <v>0.469773696608588</v>
       </c>
       <c r="H24">
-        <v>0.167118744581456</v>
+        <v>0.1648612055399581</v>
       </c>
       <c r="I24">
         <v>0.4203893727952895</v>
@@ -2415,13 +2415,13 @@
         <v>0.2344215023238028</v>
       </c>
       <c r="O24">
-        <v>0.06806721577069377</v>
+        <v>0.08376128976985853</v>
       </c>
       <c r="P24">
         <v>0.4026988190641543</v>
       </c>
       <c r="Q24">
-        <v>0.3028899548277057</v>
+        <v>0.3082769415170779</v>
       </c>
       <c r="R24">
         <v>0.2546362214002177</v>
@@ -2439,10 +2439,10 @@
         <v>0.213228980230195</v>
       </c>
       <c r="W24">
-        <v>0.2950441056285603</v>
+        <v>0.3116652659886188</v>
       </c>
       <c r="Y24">
-        <v>0.655038399630392</v>
+        <v>0.6627066721503289</v>
       </c>
       <c r="Z24">
         <v>0.8903445549760043</v>
@@ -2461,82 +2461,82 @@
         </is>
       </c>
       <c r="B25">
-        <v>0.4121078830032697</v>
+        <v>0.4147640830302365</v>
       </c>
       <c r="C25">
-        <v>0.3882268416815529</v>
+        <v>0.3987236269779414</v>
       </c>
       <c r="D25">
-        <v>0.3380533127727982</v>
+        <v>0.3311647159033571</v>
       </c>
       <c r="E25">
-        <v>0.3745608377052729</v>
+        <v>0.375047223756918</v>
       </c>
       <c r="F25">
-        <v>0.3585951886045599</v>
+        <v>0.3660074469456079</v>
       </c>
       <c r="G25">
-        <v>0.7849660069635523</v>
+        <v>0.8045217090672854</v>
       </c>
       <c r="H25">
-        <v>0.1484682200984068</v>
+        <v>0.1501384835258873</v>
       </c>
       <c r="I25">
-        <v>0.3993910979703796</v>
+        <v>0.3995156128751827</v>
       </c>
       <c r="J25">
-        <v>0.3646221304709235</v>
+        <v>0.3639976909010245</v>
       </c>
       <c r="K25">
-        <v>0.263296988813303</v>
+        <v>0.2624880755695151</v>
       </c>
       <c r="L25">
-        <v>0.2426416938901234</v>
+        <v>0.2396702670209695</v>
       </c>
       <c r="M25">
-        <v>0.2098212833323626</v>
+        <v>0.209351249320094</v>
       </c>
       <c r="N25">
-        <v>0.2064034817014902</v>
+        <v>0.20516076838721</v>
       </c>
       <c r="O25">
-        <v>0.07023256420821834</v>
+        <v>0.08081703698659988</v>
       </c>
       <c r="P25">
-        <v>0.4293052952424644</v>
+        <v>0.4345783050997502</v>
       </c>
       <c r="Q25">
-        <v>0.2912993446265165</v>
+        <v>0.3022942318695974</v>
       </c>
       <c r="R25">
-        <v>0.1765187466263051</v>
+        <v>0.181958816909036</v>
       </c>
       <c r="S25">
-        <v>0.2232979146494285</v>
+        <v>0.2294283773148871</v>
       </c>
       <c r="T25">
-        <v>0.307469395749483</v>
+        <v>0.313423316448216</v>
       </c>
       <c r="U25">
-        <v>0.1149070673411441</v>
+        <v>0.1145405512611248</v>
       </c>
       <c r="V25">
-        <v>0.2063582199614536</v>
+        <v>0.2049644406841535</v>
       </c>
       <c r="W25">
-        <v>0.2101373046847962</v>
+        <v>0.2732065978799744</v>
       </c>
       <c r="X25">
-        <v>0.655038399630392</v>
+        <v>0.6627066721503289</v>
       </c>
       <c r="Z25">
-        <v>0.7238269317650146</v>
+        <v>0.7370306800128992</v>
       </c>
       <c r="AA25">
-        <v>0.6719216750581058</v>
+        <v>0.6802556888639579</v>
       </c>
       <c r="AB25">
-        <v>0.6826332384779109</v>
+        <v>0.6960929687178846</v>
       </c>
     </row>
     <row r="26">
@@ -2561,10 +2561,10 @@
         <v>0.4339741721117608</v>
       </c>
       <c r="G26">
-        <v>0.4859926063769347</v>
+        <v>0.5454359547554969</v>
       </c>
       <c r="H26">
-        <v>0.2110968508457275</v>
+        <v>0.2107718546467774</v>
       </c>
       <c r="I26">
         <v>0.4548509819244133</v>
@@ -2585,13 +2585,13 @@
         <v>0.2096149304223076</v>
       </c>
       <c r="O26">
-        <v>0.03739180388502106</v>
+        <v>0.05511792127583255</v>
       </c>
       <c r="P26">
         <v>0.3867402416113038</v>
       </c>
       <c r="Q26">
-        <v>0.321152607530685</v>
+        <v>0.3287255710913217</v>
       </c>
       <c r="R26">
         <v>0.3021549368649482</v>
@@ -2609,13 +2609,13 @@
         <v>0.2226469068559747</v>
       </c>
       <c r="W26">
-        <v>0.3155068272502439</v>
+        <v>0.3279898868767614</v>
       </c>
       <c r="X26">
         <v>0.8903445549760043</v>
       </c>
       <c r="Y26">
-        <v>0.7238269317650146</v>
+        <v>0.7370306800128992</v>
       </c>
       <c r="AA26">
         <v>0.8752832084666128</v>
@@ -2646,10 +2646,10 @@
         <v>0.4021799804074211</v>
       </c>
       <c r="G27">
-        <v>0.4528490542911307</v>
+        <v>0.4998591441028649</v>
       </c>
       <c r="H27">
-        <v>0.1610634092400903</v>
+        <v>0.1574077995753776</v>
       </c>
       <c r="I27">
         <v>0.4403050500102345</v>
@@ -2670,13 +2670,13 @@
         <v>0.2595878516039381</v>
       </c>
       <c r="O27">
-        <v>0.08981542741864301</v>
+        <v>0.1097013220610039</v>
       </c>
       <c r="P27">
         <v>0.4368541251507124</v>
       </c>
       <c r="Q27">
-        <v>0.3171560124960915</v>
+        <v>0.3254635300179367</v>
       </c>
       <c r="R27">
         <v>0.2708006212946851</v>
@@ -2694,13 +2694,13 @@
         <v>0.2105321005094401</v>
       </c>
       <c r="W27">
-        <v>0.2827217292141312</v>
+        <v>0.2971741056403512</v>
       </c>
       <c r="X27">
         <v>0.9540884319430374</v>
       </c>
       <c r="Y27">
-        <v>0.6719216750581058</v>
+        <v>0.6802556888639579</v>
       </c>
       <c r="Z27">
         <v>0.8752832084666128</v>
@@ -2731,10 +2731,10 @@
         <v>0.3257884068861948</v>
       </c>
       <c r="G28">
-        <v>0.4851276754370418</v>
+        <v>0.5296781271196432</v>
       </c>
       <c r="H28">
-        <v>0.09538601469481374</v>
+        <v>0.08336182079441845</v>
       </c>
       <c r="I28">
         <v>0.4610309462425894</v>
@@ -2755,13 +2755,13 @@
         <v>0.2472603294569372</v>
       </c>
       <c r="O28">
-        <v>0.06216594163126758</v>
+        <v>0.07060253827758957</v>
       </c>
       <c r="P28">
         <v>0.3723707059350114</v>
       </c>
       <c r="Q28">
-        <v>0.2482325913431211</v>
+        <v>0.2535248071666839</v>
       </c>
       <c r="R28">
         <v>0.2540893277464856</v>
@@ -2779,13 +2779,13 @@
         <v>0.2028907417375988</v>
       </c>
       <c r="W28">
-        <v>0.2913500539044127</v>
+        <v>0.3006944690630143</v>
       </c>
       <c r="X28">
         <v>0.711506700631415</v>
       </c>
       <c r="Y28">
-        <v>0.6826332384779109</v>
+        <v>0.6960929687178846</v>
       </c>
       <c r="Z28">
         <v>0.7053103115923237</v>

</xml_diff>

<commit_message>
making small edits with annotations
</commit_message>
<xml_diff>
--- a/correlation_data_full.xlsx
+++ b/correlation_data_full.xlsx
@@ -506,13 +506,13 @@
         </is>
       </c>
       <c r="C2">
-        <v>0.2504501141670985</v>
+        <v>0.2504501141670986</v>
       </c>
       <c r="D2">
         <v>0.1560436763458861</v>
       </c>
       <c r="E2">
-        <v>0.0362618943639716</v>
+        <v>0.03626189436397159</v>
       </c>
       <c r="F2">
         <v>0.3353035436244038</v>
@@ -521,7 +521,7 @@
         <v>0.3369063265926281</v>
       </c>
       <c r="H2">
-        <v>-0.02759663382889261</v>
+        <v>-0.02759663382889259</v>
       </c>
       <c r="I2">
         <v>0.8962132468714507</v>
@@ -539,16 +539,16 @@
         <v>0.421497118288005</v>
       </c>
       <c r="N2">
-        <v>0.4135145171964408</v>
+        <v>0.4135145171964407</v>
       </c>
       <c r="O2">
-        <v>0.05978041870211162</v>
+        <v>0.05978041870211161</v>
       </c>
       <c r="P2">
         <v>0.2277054854577264</v>
       </c>
       <c r="Q2">
-        <v>0.0395634327022626</v>
+        <v>0.03956343270226261</v>
       </c>
       <c r="R2">
         <v>0.2213858907085259</v>
@@ -575,7 +575,7 @@
         <v>0.4147640830302365</v>
       </c>
       <c r="Z2">
-        <v>0.4439684890732144</v>
+        <v>0.4439684890732145</v>
       </c>
       <c r="AA2">
         <v>0.4396399602828737</v>
@@ -591,13 +591,13 @@
         </is>
       </c>
       <c r="B3">
-        <v>0.2504501141670985</v>
+        <v>0.2504501141670986</v>
       </c>
       <c r="D3">
         <v>0.2220463438131529</v>
       </c>
       <c r="E3">
-        <v>0.2589882165716723</v>
+        <v>0.2589882165716724</v>
       </c>
       <c r="F3">
         <v>0.3032054674842555</v>
@@ -606,19 +606,19 @@
         <v>0.3642628980363894</v>
       </c>
       <c r="H3">
-        <v>0.04435678048361254</v>
+        <v>0.04435678048361256</v>
       </c>
       <c r="I3">
-        <v>0.2550760362606682</v>
+        <v>0.2550760362606683</v>
       </c>
       <c r="J3">
-        <v>0.2355100635389874</v>
+        <v>0.2355100635389875</v>
       </c>
       <c r="K3">
         <v>0.1417578490238693</v>
       </c>
       <c r="L3">
-        <v>0.1376612696948288</v>
+        <v>0.1376612696948289</v>
       </c>
       <c r="M3">
         <v>0.1203247618736048</v>
@@ -627,7 +627,7 @@
         <v>0.1213179227496275</v>
       </c>
       <c r="O3">
-        <v>0.08229046563433723</v>
+        <v>0.0822904656343372</v>
       </c>
       <c r="P3">
         <v>0.3011142612197973</v>
@@ -651,7 +651,7 @@
         <v>0.04270461594735719</v>
       </c>
       <c r="W3">
-        <v>0.07518881647752934</v>
+        <v>0.07518881647752937</v>
       </c>
       <c r="X3">
         <v>0.4503507050477632</v>
@@ -666,7 +666,7 @@
         <v>0.4921496161070058</v>
       </c>
       <c r="AB3">
-        <v>0.4449694344044621</v>
+        <v>0.4449694344044622</v>
       </c>
     </row>
     <row r="4">
@@ -694,7 +694,7 @@
         <v>0.1966794590637176</v>
       </c>
       <c r="I4">
-        <v>0.2257782358420033</v>
+        <v>0.2257782358420032</v>
       </c>
       <c r="J4">
         <v>0.1695741123063069</v>
@@ -703,7 +703,7 @@
         <v>-0.01991398570375038</v>
       </c>
       <c r="L4">
-        <v>-0.0565600227370593</v>
+        <v>-0.05656002273705929</v>
       </c>
       <c r="M4">
         <v>0.2952574023671488</v>
@@ -718,7 +718,7 @@
         <v>0.5461144914187797</v>
       </c>
       <c r="Q4">
-        <v>0.5441676452902511</v>
+        <v>0.5441676452902512</v>
       </c>
       <c r="R4">
         <v>-0.1240677449488455</v>
@@ -761,10 +761,10 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.0362618943639716</v>
+        <v>0.03626189436397159</v>
       </c>
       <c r="C5">
-        <v>0.2589882165716723</v>
+        <v>0.2589882165716724</v>
       </c>
       <c r="D5">
         <v>0.8933567801407576</v>
@@ -782,7 +782,7 @@
         <v>0.1164079160348563</v>
       </c>
       <c r="J5">
-        <v>0.05132365040150085</v>
+        <v>0.05132365040150084</v>
       </c>
       <c r="K5">
         <v>-0.117004729312769</v>
@@ -803,13 +803,13 @@
         <v>0.5086589493774576</v>
       </c>
       <c r="Q5">
-        <v>0.6019254209528716</v>
+        <v>0.6019254209528717</v>
       </c>
       <c r="R5">
         <v>-0.0918962480429867</v>
       </c>
       <c r="S5">
-        <v>-0.03210393587441602</v>
+        <v>-0.03210393587441603</v>
       </c>
       <c r="T5">
         <v>0.560202259159532</v>
@@ -861,7 +861,7 @@
         <v>0.3502331002612809</v>
       </c>
       <c r="H6">
-        <v>-0.0346491989303611</v>
+        <v>-0.03464919893036109</v>
       </c>
       <c r="I6">
         <v>0.3308874443691532</v>
@@ -882,7 +882,7 @@
         <v>0.08909260643959102</v>
       </c>
       <c r="O6">
-        <v>0.06530966786775173</v>
+        <v>0.06530966786775175</v>
       </c>
       <c r="P6">
         <v>0.2122622921001213</v>
@@ -903,10 +903,10 @@
         <v>0.1574296744346301</v>
       </c>
       <c r="V6">
-        <v>0.01263025020116457</v>
+        <v>0.01263025020116459</v>
       </c>
       <c r="W6">
-        <v>0.07452776713627086</v>
+        <v>0.07452776713627088</v>
       </c>
       <c r="X6">
         <v>0.3827171378420469</v>
@@ -946,13 +946,13 @@
         <v>0.3502331002612809</v>
       </c>
       <c r="H7">
-        <v>0.02842854742900396</v>
+        <v>0.02842854742900395</v>
       </c>
       <c r="I7">
-        <v>0.2990948378136545</v>
+        <v>0.2990948378136546</v>
       </c>
       <c r="J7">
-        <v>0.2807759031282003</v>
+        <v>0.2807759031282002</v>
       </c>
       <c r="K7">
         <v>0.2840139339639582</v>
@@ -961,10 +961,10 @@
         <v>0.277701799782818</v>
       </c>
       <c r="M7">
-        <v>0.07440409671582113</v>
+        <v>0.07440409671582111</v>
       </c>
       <c r="N7">
-        <v>0.07013454886547639</v>
+        <v>0.0701345488654764</v>
       </c>
       <c r="O7">
         <v>0.01228480365016764</v>
@@ -988,7 +988,7 @@
         <v>0.1801322213206275</v>
       </c>
       <c r="V7">
-        <v>0.01325754104619871</v>
+        <v>0.01325754104619868</v>
       </c>
       <c r="W7">
         <v>-0.2363991004814481</v>
@@ -1016,10 +1016,10 @@
         </is>
       </c>
       <c r="B8">
-        <v>-0.02759663382889261</v>
+        <v>-0.02759663382889259</v>
       </c>
       <c r="C8">
-        <v>0.04435678048361254</v>
+        <v>0.04435678048361256</v>
       </c>
       <c r="D8">
         <v>0.1966794590637176</v>
@@ -1028,16 +1028,16 @@
         <v>0.285477589184833</v>
       </c>
       <c r="F8">
-        <v>-0.0346491989303611</v>
+        <v>-0.03464919893036109</v>
       </c>
       <c r="G8">
-        <v>0.02842854742900396</v>
+        <v>0.02842854742900395</v>
       </c>
       <c r="I8">
-        <v>-0.02341978667370561</v>
+        <v>-0.0234197866737056</v>
       </c>
       <c r="J8">
-        <v>-0.08063386203089389</v>
+        <v>-0.0806338620308939</v>
       </c>
       <c r="K8">
         <v>-0.1234323232961675</v>
@@ -1046,13 +1046,13 @@
         <v>-0.1194013037897156</v>
       </c>
       <c r="M8">
-        <v>-0.07434571563573382</v>
+        <v>-0.07434571563573383</v>
       </c>
       <c r="N8">
-        <v>-0.07287921669042526</v>
+        <v>-0.07287921669042528</v>
       </c>
       <c r="O8">
-        <v>0.01386612412697811</v>
+        <v>0.0138661241269781</v>
       </c>
       <c r="P8">
         <v>0.2774148975252184</v>
@@ -1073,10 +1073,10 @@
         <v>-0.2262761290344947</v>
       </c>
       <c r="V8">
-        <v>0.05754428796409604</v>
+        <v>0.05754428796409603</v>
       </c>
       <c r="W8">
-        <v>0.04673302774292012</v>
+        <v>0.04673302774292015</v>
       </c>
       <c r="X8">
         <v>0.1648612055399581</v>
@@ -1091,7 +1091,7 @@
         <v>0.1574077995753776</v>
       </c>
       <c r="AB8">
-        <v>0.08336182079441845</v>
+        <v>0.08336182079441846</v>
       </c>
     </row>
     <row r="9">
@@ -1104,10 +1104,10 @@
         <v>0.8962132468714507</v>
       </c>
       <c r="C9">
-        <v>0.2550760362606682</v>
+        <v>0.2550760362606683</v>
       </c>
       <c r="D9">
-        <v>0.2257782358420033</v>
+        <v>0.2257782358420032</v>
       </c>
       <c r="E9">
         <v>0.1164079160348563</v>
@@ -1116,10 +1116,10 @@
         <v>0.3308874443691532</v>
       </c>
       <c r="G9">
-        <v>0.2990948378136545</v>
+        <v>0.2990948378136546</v>
       </c>
       <c r="H9">
-        <v>-0.02341978667370561</v>
+        <v>-0.0234197866737056</v>
       </c>
       <c r="J9">
         <v>0.9712376187738408</v>
@@ -1134,16 +1134,16 @@
         <v>0.4311387230466044</v>
       </c>
       <c r="N9">
-        <v>0.4221636708752149</v>
+        <v>0.4221636708752148</v>
       </c>
       <c r="O9">
-        <v>0.09330207095356544</v>
+        <v>0.09330207095356545</v>
       </c>
       <c r="P9">
         <v>0.2568221946204033</v>
       </c>
       <c r="Q9">
-        <v>0.09287306121429487</v>
+        <v>0.09287306121429489</v>
       </c>
       <c r="R9">
         <v>0.1908115306086125</v>
@@ -1189,22 +1189,22 @@
         <v>0.8869066548957314</v>
       </c>
       <c r="C10">
-        <v>0.2355100635389874</v>
+        <v>0.2355100635389875</v>
       </c>
       <c r="D10">
         <v>0.1695741123063069</v>
       </c>
       <c r="E10">
-        <v>0.05132365040150085</v>
+        <v>0.05132365040150084</v>
       </c>
       <c r="F10">
         <v>0.3083242242546798</v>
       </c>
       <c r="G10">
-        <v>0.2807759031282003</v>
+        <v>0.2807759031282002</v>
       </c>
       <c r="H10">
-        <v>-0.08063386203089389</v>
+        <v>-0.0806338620308939</v>
       </c>
       <c r="I10">
         <v>0.9712376187738408</v>
@@ -1237,7 +1237,7 @@
         <v>0.1838740132833975</v>
       </c>
       <c r="T10">
-        <v>0.009466718180983732</v>
+        <v>0.009466718180983722</v>
       </c>
       <c r="U10">
         <v>0.2944477371716243</v>
@@ -1307,13 +1307,13 @@
         <v>0.1927308280386089</v>
       </c>
       <c r="O11">
-        <v>0.0637292450642422</v>
+        <v>0.06372924506424221</v>
       </c>
       <c r="P11">
-        <v>0.09969716055863168</v>
+        <v>0.09969716055863169</v>
       </c>
       <c r="Q11">
-        <v>-0.04759887357887706</v>
+        <v>-0.04759887357887704</v>
       </c>
       <c r="R11">
         <v>0.1484653638711309</v>
@@ -1322,7 +1322,7 @@
         <v>0.1419493414715042</v>
       </c>
       <c r="T11">
-        <v>-0.06089198647750246</v>
+        <v>-0.06089198647750245</v>
       </c>
       <c r="U11">
         <v>0.218405064445904</v>
@@ -1331,10 +1331,10 @@
         <v>0.1145027921456115</v>
       </c>
       <c r="W11">
-        <v>0.01439023441647101</v>
+        <v>0.01439023441647099</v>
       </c>
       <c r="X11">
-        <v>0.1355090426346558</v>
+        <v>0.1355090426346559</v>
       </c>
       <c r="Y11">
         <v>0.2624880755695151</v>
@@ -1359,10 +1359,10 @@
         <v>0.4801512826445933</v>
       </c>
       <c r="C12">
-        <v>0.1376612696948288</v>
+        <v>0.1376612696948289</v>
       </c>
       <c r="D12">
-        <v>-0.0565600227370593</v>
+        <v>-0.05656002273705929</v>
       </c>
       <c r="E12">
         <v>-0.1641375756109109</v>
@@ -1407,7 +1407,7 @@
         <v>0.110689173661287</v>
       </c>
       <c r="T12">
-        <v>-0.04969761963597166</v>
+        <v>-0.04969761963597168</v>
       </c>
       <c r="U12">
         <v>0.22227748487964</v>
@@ -1416,7 +1416,7 @@
         <v>0.1169420100048394</v>
       </c>
       <c r="W12">
-        <v>-0.005663670117834274</v>
+        <v>-0.005663670117834294</v>
       </c>
       <c r="X12">
         <v>0.105931356113506</v>
@@ -1425,13 +1425,13 @@
         <v>0.2396702670209695</v>
       </c>
       <c r="Z12">
-        <v>0.09475061337807365</v>
+        <v>0.09475061337807367</v>
       </c>
       <c r="AA12">
-        <v>0.1417871818067766</v>
+        <v>0.1417871818067765</v>
       </c>
       <c r="AB12">
-        <v>0.1845936274901514</v>
+        <v>0.1845936274901515</v>
       </c>
     </row>
     <row r="13">
@@ -1456,10 +1456,10 @@
         <v>0.09301441959147191</v>
       </c>
       <c r="G13">
-        <v>0.07440409671582113</v>
+        <v>0.07440409671582111</v>
       </c>
       <c r="H13">
-        <v>-0.07434571563573382</v>
+        <v>-0.07434571563573383</v>
       </c>
       <c r="I13">
         <v>0.4311387230466044</v>
@@ -1480,22 +1480,22 @@
         <v>0.556110920418823</v>
       </c>
       <c r="P13">
-        <v>0.4982138529267472</v>
+        <v>0.4982138529267473</v>
       </c>
       <c r="Q13">
         <v>0.1171519526717874</v>
       </c>
       <c r="R13">
-        <v>-0.03441708348787718</v>
+        <v>-0.03441708348787721</v>
       </c>
       <c r="S13">
-        <v>-0.03504207961216314</v>
+        <v>-0.03504207961216316</v>
       </c>
       <c r="T13">
         <v>0.1502627708979039</v>
       </c>
       <c r="U13">
-        <v>0.09167169792894313</v>
+        <v>0.09167169792894311</v>
       </c>
       <c r="V13">
         <v>0.2308717480747141</v>
@@ -1513,7 +1513,7 @@
         <v>0.2171166148616001</v>
       </c>
       <c r="AA13">
-        <v>0.2634258936300762</v>
+        <v>0.2634258936300761</v>
       </c>
       <c r="AB13">
         <v>0.2561537760680311</v>
@@ -1526,7 +1526,7 @@
         </is>
       </c>
       <c r="B14">
-        <v>0.4135145171964408</v>
+        <v>0.4135145171964407</v>
       </c>
       <c r="C14">
         <v>0.1213179227496275</v>
@@ -1541,13 +1541,13 @@
         <v>0.08909260643959102</v>
       </c>
       <c r="G14">
-        <v>0.07013454886547639</v>
+        <v>0.0701345488654764</v>
       </c>
       <c r="H14">
-        <v>-0.07287921669042526</v>
+        <v>-0.07287921669042528</v>
       </c>
       <c r="I14">
-        <v>0.4221636708752149</v>
+        <v>0.4221636708752148</v>
       </c>
       <c r="J14">
         <v>0.4077082805258652</v>
@@ -1571,16 +1571,16 @@
         <v>0.117315129888777</v>
       </c>
       <c r="R14">
-        <v>-0.04172526642003677</v>
+        <v>-0.04172526642003679</v>
       </c>
       <c r="S14">
         <v>-0.04017403757573355</v>
       </c>
       <c r="T14">
-        <v>0.153680112528515</v>
+        <v>0.1536801125285151</v>
       </c>
       <c r="U14">
-        <v>0.08802685745852554</v>
+        <v>0.08802685745852552</v>
       </c>
       <c r="V14">
         <v>0.2314141110879342</v>
@@ -1611,10 +1611,10 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.05978041870211162</v>
+        <v>0.05978041870211161</v>
       </c>
       <c r="C15">
-        <v>0.08229046563433723</v>
+        <v>0.0822904656343372</v>
       </c>
       <c r="D15">
         <v>0.2933527664426438</v>
@@ -1623,22 +1623,22 @@
         <v>0.2224772257642394</v>
       </c>
       <c r="F15">
-        <v>0.06530966786775173</v>
+        <v>0.06530966786775175</v>
       </c>
       <c r="G15">
         <v>0.01228480365016764</v>
       </c>
       <c r="H15">
-        <v>0.01386612412697811</v>
+        <v>0.0138661241269781</v>
       </c>
       <c r="I15">
-        <v>0.09330207095356544</v>
+        <v>0.09330207095356545</v>
       </c>
       <c r="J15">
         <v>0.0709232024722083</v>
       </c>
       <c r="K15">
-        <v>0.0637292450642422</v>
+        <v>0.06372924506424221</v>
       </c>
       <c r="L15">
         <v>0.06187490279114954</v>
@@ -1653,7 +1653,7 @@
         <v>0.4378019468062452</v>
       </c>
       <c r="Q15">
-        <v>0.2415135358589916</v>
+        <v>0.2415135358589917</v>
       </c>
       <c r="R15">
         <v>-0.1525669431901946</v>
@@ -1680,7 +1680,7 @@
         <v>0.08081703698659988</v>
       </c>
       <c r="Z15">
-        <v>0.05511792127583255</v>
+        <v>0.05511792127583254</v>
       </c>
       <c r="AA15">
         <v>0.1097013220610039</v>
@@ -1723,13 +1723,13 @@
         <v>0.2007180287572574</v>
       </c>
       <c r="K16">
-        <v>0.09969716055863168</v>
+        <v>0.09969716055863169</v>
       </c>
       <c r="L16">
         <v>0.1041883253381078</v>
       </c>
       <c r="M16">
-        <v>0.4982138529267472</v>
+        <v>0.4982138529267473</v>
       </c>
       <c r="N16">
         <v>0.5073508488973718</v>
@@ -1738,13 +1738,13 @@
         <v>0.4378019468062452</v>
       </c>
       <c r="Q16">
-        <v>0.8081860151953411</v>
+        <v>0.8081860151953412</v>
       </c>
       <c r="R16">
         <v>-0.1014788246072017</v>
       </c>
       <c r="S16">
-        <v>-0.03615342245176581</v>
+        <v>-0.03615342245176578</v>
       </c>
       <c r="T16">
         <v>0.8641310656617663</v>
@@ -1781,16 +1781,16 @@
         </is>
       </c>
       <c r="B17">
-        <v>0.0395634327022626</v>
+        <v>0.03956343270226261</v>
       </c>
       <c r="C17">
         <v>0.2567708194717432</v>
       </c>
       <c r="D17">
-        <v>0.5441676452902511</v>
+        <v>0.5441676452902512</v>
       </c>
       <c r="E17">
-        <v>0.6019254209528716</v>
+        <v>0.6019254209528717</v>
       </c>
       <c r="F17">
         <v>0.1756102404887688</v>
@@ -1802,13 +1802,13 @@
         <v>0.3628242646819061</v>
       </c>
       <c r="I17">
-        <v>0.09287306121429487</v>
+        <v>0.09287306121429489</v>
       </c>
       <c r="J17">
         <v>0.02295938913463506</v>
       </c>
       <c r="K17">
-        <v>-0.04759887357887706</v>
+        <v>-0.04759887357887704</v>
       </c>
       <c r="L17">
         <v>-0.07981620181669503</v>
@@ -1820,10 +1820,10 @@
         <v>0.117315129888777</v>
       </c>
       <c r="O17">
-        <v>0.2415135358589916</v>
+        <v>0.2415135358589917</v>
       </c>
       <c r="P17">
-        <v>0.8081860151953411</v>
+        <v>0.8081860151953412</v>
       </c>
       <c r="R17">
         <v>-0.1730404339624289</v>
@@ -1832,7 +1832,7 @@
         <v>-0.1060010172985709</v>
       </c>
       <c r="T17">
-        <v>0.9452761297779024</v>
+        <v>0.9452761297779023</v>
       </c>
       <c r="U17">
         <v>-0.1807436460765975</v>
@@ -1899,10 +1899,10 @@
         <v>0.1191647463280724</v>
       </c>
       <c r="M18">
-        <v>-0.03441708348787718</v>
+        <v>-0.03441708348787721</v>
       </c>
       <c r="N18">
-        <v>-0.04172526642003677</v>
+        <v>-0.04172526642003679</v>
       </c>
       <c r="O18">
         <v>-0.1525669431901946</v>
@@ -1960,7 +1960,7 @@
         <v>-0.07442091165502744</v>
       </c>
       <c r="E19">
-        <v>-0.03210393587441602</v>
+        <v>-0.03210393587441603</v>
       </c>
       <c r="F19">
         <v>0.326391697294726</v>
@@ -1984,7 +1984,7 @@
         <v>0.110689173661287</v>
       </c>
       <c r="M19">
-        <v>-0.03504207961216314</v>
+        <v>-0.03504207961216316</v>
       </c>
       <c r="N19">
         <v>-0.04017403757573355</v>
@@ -1993,7 +1993,7 @@
         <v>-0.105669554314247</v>
       </c>
       <c r="P19">
-        <v>-0.03615342245176581</v>
+        <v>-0.03615342245176578</v>
       </c>
       <c r="Q19">
         <v>-0.1060010172985709</v>
@@ -2011,7 +2011,7 @@
         <v>-0.0928560701431425</v>
       </c>
       <c r="W19">
-        <v>0.06754019836006939</v>
+        <v>0.0675401983600694</v>
       </c>
       <c r="X19">
         <v>0.2811295216726082</v>
@@ -2060,19 +2060,19 @@
         <v>0.07218036953787371</v>
       </c>
       <c r="J20">
-        <v>0.009466718180983732</v>
+        <v>0.009466718180983722</v>
       </c>
       <c r="K20">
-        <v>-0.06089198647750246</v>
+        <v>-0.06089198647750245</v>
       </c>
       <c r="L20">
-        <v>-0.04969761963597166</v>
+        <v>-0.04969761963597168</v>
       </c>
       <c r="M20">
         <v>0.1502627708979039</v>
       </c>
       <c r="N20">
-        <v>0.153680112528515</v>
+        <v>0.1536801125285151</v>
       </c>
       <c r="O20">
         <v>0.2679599545219127</v>
@@ -2081,7 +2081,7 @@
         <v>0.8641310656617663</v>
       </c>
       <c r="Q20">
-        <v>0.9452761297779024</v>
+        <v>0.9452761297779023</v>
       </c>
       <c r="R20">
         <v>-0.1694610076243347</v>
@@ -2099,7 +2099,7 @@
         <v>0.1653826925730575</v>
       </c>
       <c r="X20">
-        <v>0.2918502019583458</v>
+        <v>0.2918502019583457</v>
       </c>
       <c r="Y20">
         <v>0.313423316448216</v>
@@ -2154,10 +2154,10 @@
         <v>0.22227748487964</v>
       </c>
       <c r="M21">
-        <v>0.09167169792894313</v>
+        <v>0.09167169792894311</v>
       </c>
       <c r="N21">
-        <v>0.08802685745852554</v>
+        <v>0.08802685745852552</v>
       </c>
       <c r="O21">
         <v>-0.1003708712144724</v>
@@ -2178,10 +2178,10 @@
         <v>-0.2198006607497221</v>
       </c>
       <c r="V21">
-        <v>0.0009227254258041933</v>
+        <v>0.0009227254258042129</v>
       </c>
       <c r="W21">
-        <v>0.01675869359039526</v>
+        <v>0.01675869359039527</v>
       </c>
       <c r="X21">
         <v>0.2811474278249858</v>
@@ -2196,7 +2196,7 @@
         <v>0.3104956334922062</v>
       </c>
       <c r="AB21">
-        <v>0.2930197519048968</v>
+        <v>0.2930197519048969</v>
       </c>
     </row>
     <row r="22">
@@ -2218,13 +2218,13 @@
         <v>0.2266480702911372</v>
       </c>
       <c r="F22">
-        <v>0.01263025020116457</v>
+        <v>0.01263025020116459</v>
       </c>
       <c r="G22">
-        <v>0.01325754104619871</v>
+        <v>0.01325754104619868</v>
       </c>
       <c r="H22">
-        <v>0.05754428796409604</v>
+        <v>0.05754428796409603</v>
       </c>
       <c r="I22">
         <v>0.2124414934558372</v>
@@ -2263,7 +2263,7 @@
         <v>0.1261521508710033</v>
       </c>
       <c r="U22">
-        <v>0.0009227254258041933</v>
+        <v>0.0009227254258042129</v>
       </c>
       <c r="W22">
         <v>0.3635434921086566</v>
@@ -2272,13 +2272,13 @@
         <v>0.213228980230195</v>
       </c>
       <c r="Y22">
-        <v>0.2049644406841535</v>
+        <v>0.2049644406841534</v>
       </c>
       <c r="Z22">
         <v>0.2226469068559747</v>
       </c>
       <c r="AA22">
-        <v>0.2105321005094401</v>
+        <v>0.21053210050944</v>
       </c>
       <c r="AB22">
         <v>0.2028907417375988</v>
@@ -2294,7 +2294,7 @@
         <v>0.1877658152845463</v>
       </c>
       <c r="C23">
-        <v>0.07518881647752934</v>
+        <v>0.07518881647752937</v>
       </c>
       <c r="D23">
         <v>0.3999202176911701</v>
@@ -2303,13 +2303,13 @@
         <v>0.3457429837212002</v>
       </c>
       <c r="F23">
-        <v>0.07452776713627086</v>
+        <v>0.07452776713627088</v>
       </c>
       <c r="G23">
         <v>-0.2363991004814481</v>
       </c>
       <c r="H23">
-        <v>0.04673302774292012</v>
+        <v>0.04673302774292015</v>
       </c>
       <c r="I23">
         <v>0.2332344048041308</v>
@@ -2318,10 +2318,10 @@
         <v>0.2174749294945283</v>
       </c>
       <c r="K23">
-        <v>0.01439023441647101</v>
+        <v>0.01439023441647099</v>
       </c>
       <c r="L23">
-        <v>-0.005663670117834274</v>
+        <v>-0.005663670117834294</v>
       </c>
       <c r="M23">
         <v>0.2231103204226994</v>
@@ -2342,13 +2342,13 @@
         <v>0.09390252887980635</v>
       </c>
       <c r="S23">
-        <v>0.06754019836006939</v>
+        <v>0.0675401983600694</v>
       </c>
       <c r="T23">
         <v>0.1653826925730575</v>
       </c>
       <c r="U23">
-        <v>0.01675869359039526</v>
+        <v>0.01675869359039527</v>
       </c>
       <c r="V23">
         <v>0.3635434921086566</v>
@@ -2357,7 +2357,7 @@
         <v>0.3116652659886188</v>
       </c>
       <c r="Y23">
-        <v>0.2732065978799744</v>
+        <v>0.2732065978799743</v>
       </c>
       <c r="Z23">
         <v>0.3279898868767614</v>
@@ -2366,7 +2366,7 @@
         <v>0.2971741056403512</v>
       </c>
       <c r="AB23">
-        <v>0.3006944690630143</v>
+        <v>0.3006944690630144</v>
       </c>
     </row>
     <row r="24">
@@ -2403,7 +2403,7 @@
         <v>0.3719322857189268</v>
       </c>
       <c r="K24">
-        <v>0.1355090426346558</v>
+        <v>0.1355090426346559</v>
       </c>
       <c r="L24">
         <v>0.105931356113506</v>
@@ -2430,7 +2430,7 @@
         <v>0.2811295216726082</v>
       </c>
       <c r="T24">
-        <v>0.2918502019583458</v>
+        <v>0.2918502019583457</v>
       </c>
       <c r="U24">
         <v>0.2811474278249858</v>
@@ -2521,10 +2521,10 @@
         <v>0.1145405512611248</v>
       </c>
       <c r="V25">
-        <v>0.2049644406841535</v>
+        <v>0.2049644406841534</v>
       </c>
       <c r="W25">
-        <v>0.2732065978799744</v>
+        <v>0.2732065978799743</v>
       </c>
       <c r="X25">
         <v>0.6627066721503289</v>
@@ -2533,7 +2533,7 @@
         <v>0.7370306800128992</v>
       </c>
       <c r="AA25">
-        <v>0.6802556888639579</v>
+        <v>0.6802556888639578</v>
       </c>
       <c r="AB25">
         <v>0.6960929687178846</v>
@@ -2546,7 +2546,7 @@
         </is>
       </c>
       <c r="B26">
-        <v>0.4439684890732144</v>
+        <v>0.4439684890732145</v>
       </c>
       <c r="C26">
         <v>0.4463879454956496</v>
@@ -2576,7 +2576,7 @@
         <v>0.142712643179018</v>
       </c>
       <c r="L26">
-        <v>0.09475061337807365</v>
+        <v>0.09475061337807367</v>
       </c>
       <c r="M26">
         <v>0.2171166148616001</v>
@@ -2585,7 +2585,7 @@
         <v>0.2096149304223076</v>
       </c>
       <c r="O26">
-        <v>0.05511792127583255</v>
+        <v>0.05511792127583254</v>
       </c>
       <c r="P26">
         <v>0.3867402416113038</v>
@@ -2661,10 +2661,10 @@
         <v>0.1650434677702124</v>
       </c>
       <c r="L27">
-        <v>0.1417871818067766</v>
+        <v>0.1417871818067765</v>
       </c>
       <c r="M27">
-        <v>0.2634258936300762</v>
+        <v>0.2634258936300761</v>
       </c>
       <c r="N27">
         <v>0.2595878516039381</v>
@@ -2691,7 +2691,7 @@
         <v>0.3104956334922062</v>
       </c>
       <c r="V27">
-        <v>0.2105321005094401</v>
+        <v>0.21053210050944</v>
       </c>
       <c r="W27">
         <v>0.2971741056403512</v>
@@ -2700,7 +2700,7 @@
         <v>0.9540884319430374</v>
       </c>
       <c r="Y27">
-        <v>0.6802556888639579</v>
+        <v>0.6802556888639578</v>
       </c>
       <c r="Z27">
         <v>0.8752832084666128</v>
@@ -2719,7 +2719,7 @@
         <v>0.4632929735172144</v>
       </c>
       <c r="C28">
-        <v>0.4449694344044621</v>
+        <v>0.4449694344044622</v>
       </c>
       <c r="D28">
         <v>0.4156764728076081</v>
@@ -2734,7 +2734,7 @@
         <v>0.5296781271196432</v>
       </c>
       <c r="H28">
-        <v>0.08336182079441845</v>
+        <v>0.08336182079441846</v>
       </c>
       <c r="I28">
         <v>0.4610309462425894</v>
@@ -2746,7 +2746,7 @@
         <v>0.2129034349415712</v>
       </c>
       <c r="L28">
-        <v>0.1845936274901514</v>
+        <v>0.1845936274901515</v>
       </c>
       <c r="M28">
         <v>0.2561537760680311</v>
@@ -2773,13 +2773,13 @@
         <v>0.2348240657617434</v>
       </c>
       <c r="U28">
-        <v>0.2930197519048968</v>
+        <v>0.2930197519048969</v>
       </c>
       <c r="V28">
         <v>0.2028907417375988</v>
       </c>
       <c r="W28">
-        <v>0.3006944690630143</v>
+        <v>0.3006944690630144</v>
       </c>
       <c r="X28">
         <v>0.711506700631415</v>

</xml_diff>